<commit_message>
more work on oilcane
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_1.xlsx
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.1304144337925773</v>
+        <v>-0.1304925126117005</v>
       </c>
       <c r="D4" t="n">
         <v>-0.006983176887327074</v>
@@ -746,79 +746,79 @@
         <v>-0.0009319498932779957</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04040396734415869</v>
+        <v>0.04040429384017175</v>
       </c>
       <c r="H4" t="n">
         <v>0.1569397492215899</v>
       </c>
       <c r="I4" t="n">
-        <v>0.02483110899324436</v>
+        <v>0.02515442241417689</v>
       </c>
       <c r="J4" t="n">
-        <v>0.358111059513581</v>
+        <v>0.3572328694997604</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4308811248512449</v>
+        <v>0.2027413483656539</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4308811248512449</v>
+        <v>0.2027413483656539</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4308811248512449</v>
+        <v>0.2027413483656539</v>
       </c>
       <c r="N4" t="n">
-        <v>0.4308811248512449</v>
+        <v>0.2027413483656539</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4308811248512449</v>
+        <v>0.2027413483656539</v>
       </c>
       <c r="P4" t="n">
-        <v>0.006197271703890867</v>
+        <v>0.008892453283698131</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.2019338775493551</v>
+        <v>0.1849573781822951</v>
       </c>
       <c r="R4" t="n">
-        <v>0.2019338775493551</v>
+        <v>0.1849573781822951</v>
       </c>
       <c r="S4" t="n">
-        <v>0.2019338775493551</v>
+        <v>0.1849573781822951</v>
       </c>
       <c r="T4" t="n">
-        <v>0.2019338775493551</v>
+        <v>0.1849573781822951</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.07929377462775097</v>
+        <v>-0.07926304195452168</v>
       </c>
       <c r="V4" t="n">
         <v>-0.6985461087418442</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.00145170850606834</v>
+        <v>-0.001453123162124926</v>
       </c>
       <c r="X4" t="n">
-        <v>0.2043617088144683</v>
+        <v>0.2043617816784712</v>
       </c>
       <c r="Y4" t="n">
         <v>0.9980752059710081</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.1333571908382876</v>
+        <v>0.1334010568880423</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.05632499946899998</v>
+        <v>0.02386641666665666</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.05632499946899998</v>
+        <v>0.02386641666665666</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.05632499946899998</v>
+        <v>0.02386641666665666</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.05632499946899998</v>
+        <v>0.02386641666665666</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.05632499946899998</v>
+        <v>0.02386641666665666</v>
       </c>
     </row>
     <row r="5">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.08751003191640126</v>
+        <v>0.08750749415629976</v>
       </c>
       <c r="D5" t="n">
         <v>-0.0005059528522381141</v>
@@ -841,79 +841,79 @@
         <v>0.007442291337691653</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0927535176621407</v>
+        <v>-0.09275319087812761</v>
       </c>
       <c r="H5" t="n">
         <v>-0.007557608750304349</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0314605598504224</v>
+        <v>-0.03149860167594406</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01555388363244671</v>
+        <v>0.01476774877693747</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1783261470050459</v>
+        <v>-0.05427416290696651</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1783261470050459</v>
+        <v>-0.05427416290696651</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.1783261470050459</v>
+        <v>-0.05427416290696651</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.1783261470050459</v>
+        <v>-0.05427416290696651</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.1783261470050459</v>
+        <v>-0.05427416290696651</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02934415077376602</v>
+        <v>0.0309628374625135</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.1228959032838361</v>
+        <v>-0.09038812470352499</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.1228959032838361</v>
+        <v>-0.09038812470352499</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.1228959032838361</v>
+        <v>-0.09038812470352499</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.1228959032838361</v>
+        <v>-0.09038812470352499</v>
       </c>
       <c r="U5" t="n">
-        <v>0.08792990943719636</v>
+        <v>0.08791041874841674</v>
       </c>
       <c r="V5" t="n">
         <v>0.6494536938821477</v>
       </c>
       <c r="W5" t="n">
-        <v>0.003099321723972869</v>
+        <v>0.00309863426794537</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.1488095743683829</v>
+        <v>-0.1488094079043763</v>
       </c>
       <c r="Y5" t="n">
         <v>-0.0003607808784312351</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.08921481198459247</v>
+        <v>-0.08903257440930297</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.07498515285540611</v>
+        <v>-0.06878231603129263</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.07498515285540611</v>
+        <v>-0.06878231603129263</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.07498515285540611</v>
+        <v>-0.06878231603129263</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.07498515285540611</v>
+        <v>-0.06878231603129263</v>
       </c>
       <c r="AE5" t="n">
-        <v>-0.07498515285540611</v>
+        <v>-0.06878231603129263</v>
       </c>
     </row>
     <row r="6">
@@ -924,7 +924,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2096388536015541</v>
+        <v>0.2096535558101422</v>
       </c>
       <c r="D6" t="n">
         <v>0.9579628848145153</v>
@@ -936,79 +936,79 @@
         <v>0.02074190137367605</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.004640998937639957</v>
+        <v>-0.004640835353633414</v>
       </c>
       <c r="H6" t="n">
         <v>-0.0210553376422135</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9105516352700652</v>
+        <v>0.9105359745014389</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.1784454950916717</v>
+        <v>-0.1792069637265501</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.01507945855517834</v>
+        <v>-0.0004290222891608915</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.01507945855517834</v>
+        <v>-0.0004290222891608915</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.01507945855517834</v>
+        <v>-0.0004290222891608915</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.01507945855517834</v>
+        <v>-0.0004290222891608915</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.01507945855517834</v>
+        <v>-0.0004290222891608915</v>
       </c>
       <c r="P6" t="n">
-        <v>0.01186293733851749</v>
+        <v>0.01328820725152829</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.01114219369368774</v>
+        <v>0.01481230340849213</v>
       </c>
       <c r="R6" t="n">
-        <v>0.01114219369368774</v>
+        <v>0.01481230340849213</v>
       </c>
       <c r="S6" t="n">
-        <v>0.01114219369368774</v>
+        <v>0.01481230340849213</v>
       </c>
       <c r="T6" t="n">
-        <v>0.01114219369368774</v>
+        <v>0.01481230340849213</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0009129969005198759</v>
+        <v>0.0008974494118979764</v>
       </c>
       <c r="V6" t="n">
         <v>0.0006903616596144663</v>
       </c>
       <c r="W6" t="n">
-        <v>0.02499176125567045</v>
+        <v>0.02499272874370915</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.02990583594823343</v>
+        <v>-0.02990856330834253</v>
       </c>
       <c r="Y6" t="n">
         <v>-0.00930846901233876</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.3008042411841696</v>
+        <v>0.3009131431085257</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.05302283223291328</v>
+        <v>0.04603405950536237</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.05302283223291328</v>
+        <v>0.04603405950536237</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.05302283223291328</v>
+        <v>0.04603405950536237</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.05302283223291328</v>
+        <v>0.04603405950536237</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.05302283223291328</v>
+        <v>0.04603405950536237</v>
       </c>
     </row>
     <row r="7">
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4742833735313349</v>
+        <v>0.4742883386515335</v>
       </c>
       <c r="D7" t="n">
         <v>0.001493300027732001</v>
@@ -1035,79 +1035,79 @@
         <v>-0.02376722984668919</v>
       </c>
       <c r="G7" t="n">
-        <v>0.02531693448467737</v>
+        <v>0.0253171176526847</v>
       </c>
       <c r="H7" t="n">
         <v>0.02089995155599806</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01540868346434734</v>
+        <v>0.01536951143078046</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.01628920324672423</v>
+        <v>-0.01647793139238206</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.03160303547212141</v>
+        <v>-0.02894841283793652</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.03160303547212141</v>
+        <v>-0.02894841283793652</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.03160303547212141</v>
+        <v>-0.02894841283793652</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.03160303547212141</v>
+        <v>-0.02894841283793652</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.03160303547212141</v>
+        <v>-0.02894841283793652</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.02499027181561087</v>
+        <v>-0.02596660078266403</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.02829025332361013</v>
+        <v>-0.03394260606170424</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.02829025332361013</v>
+        <v>-0.03394260606170424</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.02829025332361013</v>
+        <v>-0.03394260606170424</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.02829025332361013</v>
+        <v>-0.03394260606170424</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.5644133602725343</v>
+        <v>-0.5644336490093459</v>
       </c>
       <c r="V7" t="n">
         <v>0.02024035818561432</v>
       </c>
       <c r="W7" t="n">
-        <v>0.009486977947479117</v>
+        <v>0.009487690843507634</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.03417533522301341</v>
+        <v>-0.03418148114325924</v>
       </c>
       <c r="Y7" t="n">
         <v>-0.02165144957005798</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.02407149619485984</v>
+        <v>-0.02384080828163233</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.03155476081419042</v>
+        <v>0.0369078176043127</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.03155476081419042</v>
+        <v>0.0369078176043127</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.03155476081419042</v>
+        <v>0.0369078176043127</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.03155476081419042</v>
+        <v>0.0369078176043127</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.03155476081419042</v>
+        <v>0.0369078176043127</v>
       </c>
     </row>
     <row r="8">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5190032646961305</v>
+        <v>0.5190148800245951</v>
       </c>
       <c r="D8" t="n">
         <v>-0.009443602841744113</v>
@@ -1134,79 +1134,79 @@
         <v>-0.01173461288538451</v>
       </c>
       <c r="G8" t="n">
-        <v>0.009965621966624878</v>
+        <v>0.009965773166630923</v>
       </c>
       <c r="H8" t="n">
         <v>0.009729175493167019</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.00870311775612471</v>
+        <v>-0.008744475421779016</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.00617867737441322</v>
+        <v>-0.006548917185587564</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.004917619300704771</v>
+        <v>-0.002795285199811408</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.004917619300704771</v>
+        <v>-0.002795285199811408</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.004917619300704771</v>
+        <v>-0.002795285199811408</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.004917619300704771</v>
+        <v>-0.002795285199811408</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.004917619300704771</v>
+        <v>-0.002795285199811408</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.0107941625757665</v>
+        <v>-0.0106110125204405</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.011246300129852</v>
+        <v>-0.008121920196876806</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.011246300129852</v>
+        <v>-0.008121920196876806</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.011246300129852</v>
+        <v>-0.008121920196876806</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.011246300129852</v>
+        <v>-0.008121920196876806</v>
       </c>
       <c r="U8" t="n">
-        <v>0.6565887760875511</v>
+        <v>0.6565761310630452</v>
       </c>
       <c r="V8" t="n">
         <v>0.003534986061399442</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.01466756900270276</v>
+        <v>-0.01466622212264888</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0223501875180075</v>
+        <v>0.02235018579000743</v>
       </c>
       <c r="Y8" t="n">
         <v>-0.0137138349805534</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.01954405047776202</v>
+        <v>0.01948847578753903</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.0201475200379008</v>
+        <v>-0.01920860880034435</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.0201475200379008</v>
+        <v>-0.01920860880034435</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.0201475200379008</v>
+        <v>-0.01920860880034435</v>
       </c>
       <c r="AD8" t="n">
-        <v>-0.0201475200379008</v>
+        <v>-0.01920860880034435</v>
       </c>
       <c r="AE8" t="n">
-        <v>-0.0201475200379008</v>
+        <v>-0.01920860880034435</v>
       </c>
     </row>
     <row r="9">
@@ -1221,7 +1221,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0187947025757881</v>
+        <v>0.01880188299207532</v>
       </c>
       <c r="D9" t="n">
         <v>0.02935640968625638</v>
@@ -1233,79 +1233,79 @@
         <v>0.01226541207461648</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.00885802278632091</v>
+        <v>-0.008857972674318907</v>
       </c>
       <c r="H9" t="n">
         <v>-0.009739886885595473</v>
       </c>
       <c r="I9" t="n">
-        <v>0.02187698938707957</v>
+        <v>0.02187622369104894</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0004196461612793503</v>
+        <v>-0.0001769353033916493</v>
       </c>
       <c r="K9" t="n">
-        <v>0.006080892435235697</v>
+        <v>0.009728747237149888</v>
       </c>
       <c r="L9" t="n">
-        <v>0.006080892435235697</v>
+        <v>0.009728747237149888</v>
       </c>
       <c r="M9" t="n">
-        <v>0.006080892435235697</v>
+        <v>0.009728747237149888</v>
       </c>
       <c r="N9" t="n">
-        <v>0.006080892435235697</v>
+        <v>0.009728747237149888</v>
       </c>
       <c r="O9" t="n">
-        <v>0.006080892435235697</v>
+        <v>0.009728747237149888</v>
       </c>
       <c r="P9" t="n">
-        <v>0.01147977453919098</v>
+        <v>0.01226659431466377</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.009947735629909424</v>
+        <v>0.01270564927622597</v>
       </c>
       <c r="R9" t="n">
-        <v>0.009947735629909424</v>
+        <v>0.01270564927622597</v>
       </c>
       <c r="S9" t="n">
-        <v>0.009947735629909424</v>
+        <v>0.01270564927622597</v>
       </c>
       <c r="T9" t="n">
-        <v>0.009947735629909424</v>
+        <v>0.01270564927622597</v>
       </c>
       <c r="U9" t="n">
-        <v>0.001486497563459902</v>
+        <v>0.001513283292531331</v>
       </c>
       <c r="V9" t="n">
         <v>0.01008248142729926</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.01503771237750849</v>
+        <v>-0.01503888655355546</v>
       </c>
       <c r="X9" t="n">
-        <v>-0.003307496484299859</v>
+        <v>-0.0033043375081735</v>
       </c>
       <c r="Y9" t="n">
         <v>0.0114918274356731</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.008711337852453512</v>
+        <v>0.008479006131160243</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.000127607525104301</v>
+        <v>-0.002657999626319985</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.000127607525104301</v>
+        <v>-0.002657999626319985</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.000127607525104301</v>
+        <v>-0.002657999626319985</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.000127607525104301</v>
+        <v>-0.002657999626319985</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.000127607525104301</v>
+        <v>-0.002657999626319985</v>
       </c>
     </row>
     <row r="10">
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.06793265206130607</v>
+        <v>0.06793405250936209</v>
       </c>
       <c r="D10" t="n">
         <v>-0.0009429528377181134</v>
@@ -1332,79 +1332,79 @@
         <v>-0.00899081901563276</v>
       </c>
       <c r="G10" t="n">
-        <v>0.008694083963763357</v>
+        <v>0.008694158939766357</v>
       </c>
       <c r="H10" t="n">
         <v>0.009487848667513945</v>
       </c>
       <c r="I10" t="n">
-        <v>0.003474302634972105</v>
+        <v>0.003493966123758645</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.005670677417495813</v>
+        <v>-0.005406378465856867</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.007820831256833249</v>
+        <v>-0.01590507298820292</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.007820831256833249</v>
+        <v>-0.01590507298820292</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.007820831256833249</v>
+        <v>-0.01590507298820292</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.007820831256833249</v>
+        <v>-0.01590507298820292</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.007820831256833249</v>
+        <v>-0.01590507298820292</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.008757804830312192</v>
+        <v>-0.01003837844953514</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.008472029522881178</v>
+        <v>-0.0156722350588894</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.008472029522881178</v>
+        <v>-0.0156722350588894</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.008472029522881178</v>
+        <v>-0.0156722350588894</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.008472029522881178</v>
+        <v>-0.0156722350588894</v>
       </c>
       <c r="U10" t="n">
-        <v>0.06500410157616404</v>
+        <v>0.06496334122253364</v>
       </c>
       <c r="V10" t="n">
         <v>-0.005573894910955795</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.002946408885856355</v>
+        <v>-0.002946754677870186</v>
       </c>
       <c r="X10" t="n">
-        <v>0.01390045198001808</v>
+        <v>0.01390463652418546</v>
       </c>
       <c r="Y10" t="n">
         <v>0.005369976598799063</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.005600718848028753</v>
+        <v>0.005986437935457517</v>
       </c>
       <c r="AA10" t="n">
-        <v>-0.00884323379372935</v>
+        <v>-0.008231081033243239</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.00884323379372935</v>
+        <v>-0.008231081033243239</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.00884323379372935</v>
+        <v>-0.008231081033243239</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.00884323379372935</v>
+        <v>-0.008231081033243239</v>
       </c>
       <c r="AE10" t="n">
-        <v>-0.00884323379372935</v>
+        <v>-0.008231081033243239</v>
       </c>
     </row>
     <row r="11">
@@ -1415,7 +1415,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1556036817441472</v>
+        <v>0.1556083294883332</v>
       </c>
       <c r="D11" t="n">
         <v>0.2739322870212915</v>
@@ -1427,79 +1427,79 @@
         <v>-0.00115258574210343</v>
       </c>
       <c r="G11" t="n">
-        <v>0.003232328097293123</v>
+        <v>0.003232147905285916</v>
       </c>
       <c r="H11" t="n">
         <v>0.0004981172359246894</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.004134914661396586</v>
+        <v>-0.004123338980933559</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.01122006478199739</v>
+        <v>-0.01109784617562362</v>
       </c>
       <c r="K11" t="n">
-        <v>0.005581443199257728</v>
+        <v>0.00612064680482587</v>
       </c>
       <c r="L11" t="n">
-        <v>0.005581443199257728</v>
+        <v>0.00612064680482587</v>
       </c>
       <c r="M11" t="n">
-        <v>0.005581443199257728</v>
+        <v>0.00612064680482587</v>
       </c>
       <c r="N11" t="n">
-        <v>0.005581443199257728</v>
+        <v>0.00612064680482587</v>
       </c>
       <c r="O11" t="n">
-        <v>0.005581443199257728</v>
+        <v>0.00612064680482587</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.001394267671770707</v>
+        <v>3.765436950617478e-05</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.002917575476703019</v>
+        <v>0.003635796049431841</v>
       </c>
       <c r="R11" t="n">
-        <v>0.002917575476703019</v>
+        <v>0.003635796049431841</v>
       </c>
       <c r="S11" t="n">
-        <v>0.002917575476703019</v>
+        <v>0.003635796049431841</v>
       </c>
       <c r="T11" t="n">
-        <v>0.002917575476703019</v>
+        <v>0.003635796049431841</v>
       </c>
       <c r="U11" t="n">
-        <v>0.03581718488868739</v>
+        <v>0.0358190426807617</v>
       </c>
       <c r="V11" t="n">
         <v>-0.01363826444953058</v>
       </c>
       <c r="W11" t="n">
-        <v>-0.002545951589838063</v>
+        <v>-0.002544678437787137</v>
       </c>
       <c r="X11" t="n">
-        <v>0.0114838050033522</v>
+        <v>0.01148722682748907</v>
       </c>
       <c r="Y11" t="n">
         <v>0.0004630551545222061</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.01120140976005639</v>
+        <v>0.01113628134145125</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.005403148632125944</v>
+        <v>-0.00732070176482807</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.005403148632125944</v>
+        <v>-0.00732070176482807</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.005403148632125944</v>
+        <v>-0.00732070176482807</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.005403148632125944</v>
+        <v>-0.00732070176482807</v>
       </c>
       <c r="AE11" t="n">
-        <v>-0.005403148632125944</v>
+        <v>-0.00732070176482807</v>
       </c>
     </row>
     <row r="12">
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.277960524654421</v>
+        <v>-0.2779589221263568</v>
       </c>
       <c r="D12" t="n">
         <v>0.00596510827060433</v>
@@ -1522,79 +1522,79 @@
         <v>-0.002427315457092618</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0010758175150327</v>
+        <v>0.001075671691026868</v>
       </c>
       <c r="H12" t="n">
         <v>0.003546004461840178</v>
       </c>
       <c r="I12" t="n">
-        <v>0.006743385197735407</v>
+        <v>0.006736576301463051</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.00754548448669287</v>
+        <v>-0.007020700085296766</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.004422072752882909</v>
+        <v>-0.02114070775762831</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.004422072752882909</v>
+        <v>-0.02114070775762831</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.004422072752882909</v>
+        <v>-0.02114070775762831</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.004422072752882909</v>
+        <v>-0.02114070775762831</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.004422072752882909</v>
+        <v>-0.02114070775762831</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.002310469436418777</v>
+        <v>-0.004170422662816906</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.003192587935703517</v>
+        <v>-0.01587752645910106</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.003192587935703517</v>
+        <v>-0.01587752645910106</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.003192587935703517</v>
+        <v>-0.01587752645910106</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.003192587935703517</v>
+        <v>-0.01587752645910106</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.04390731554829261</v>
+        <v>-0.04391862482874499</v>
       </c>
       <c r="V12" t="n">
         <v>0.002068597522743901</v>
       </c>
       <c r="W12" t="n">
-        <v>-0.01060577447223098</v>
+        <v>-0.01060585914423436</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.02172128707685148</v>
+        <v>-0.02172307939692317</v>
       </c>
       <c r="Y12" t="n">
         <v>0.01261590818463632</v>
       </c>
       <c r="Z12" t="n">
-        <v>-0.01970714853228594</v>
+        <v>-0.01964870804994832</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.01609363581174543</v>
+        <v>0.01988845807553832</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.01609363581174543</v>
+        <v>0.01988845807553832</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.01609363581174543</v>
+        <v>0.01988845807553832</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.01609363581174543</v>
+        <v>0.01988845807553832</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.01609363581174543</v>
+        <v>0.01988845807553832</v>
       </c>
     </row>
     <row r="13">
@@ -1609,7 +1609,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.03300117588004703</v>
+        <v>0.03299340784773631</v>
       </c>
       <c r="D13" t="n">
         <v>0.008566614198664566</v>
@@ -1621,79 +1621,79 @@
         <v>0.0004245209449808377</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0002883188275327531</v>
+        <v>0.0002881691635267665</v>
       </c>
       <c r="H13" t="n">
         <v>0.0003968549918741996</v>
       </c>
       <c r="I13" t="n">
-        <v>0.01185593289023731</v>
+        <v>0.01186119340244773</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.006104112203342924</v>
+        <v>-0.006385798202773106</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.006020690064827601</v>
+        <v>0.01443265804930632</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.006020690064827601</v>
+        <v>0.01443265804930632</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.006020690064827601</v>
+        <v>0.01443265804930632</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.006020690064827601</v>
+        <v>0.01443265804930632</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.006020690064827601</v>
+        <v>0.01443265804930632</v>
       </c>
       <c r="P13" t="n">
-        <v>0.0003507486860299474</v>
+        <v>0.001869413162776527</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.002066624146664966</v>
+        <v>0.005577475711099028</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.002066624146664966</v>
+        <v>0.005577475711099028</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.002066624146664966</v>
+        <v>0.005577475711099028</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.002066624146664966</v>
+        <v>0.005577475711099028</v>
       </c>
       <c r="U13" t="n">
-        <v>0.03519659199986368</v>
+        <v>0.03523513264140531</v>
       </c>
       <c r="V13" t="n">
         <v>0.01221857194474288</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.01560343540813741</v>
+        <v>-0.01560367214414688</v>
       </c>
       <c r="X13" t="n">
-        <v>0.01045480640219225</v>
+        <v>0.01045741328229653</v>
       </c>
       <c r="Y13" t="n">
         <v>-0.0003000131640005266</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.01410321781212871</v>
+        <v>0.01375589776623591</v>
       </c>
       <c r="AA13" t="n">
-        <v>-0.01275319875012795</v>
+        <v>-0.01572666302906652</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.01275319875012795</v>
+        <v>-0.01572666302906652</v>
       </c>
       <c r="AC13" t="n">
-        <v>-0.01275319875012795</v>
+        <v>-0.01572666302906652</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.01275319875012795</v>
+        <v>-0.01572666302906652</v>
       </c>
       <c r="AE13" t="n">
-        <v>-0.01275319875012795</v>
+        <v>-0.01572666302906652</v>
       </c>
     </row>
     <row r="14">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.0297665724866629</v>
+        <v>-0.02977057559082302</v>
       </c>
       <c r="D14" t="n">
         <v>-0.007119685916787436</v>
@@ -1720,79 +1720,79 @@
         <v>-0.009246409425856375</v>
       </c>
       <c r="G14" t="n">
-        <v>0.008410156848406274</v>
+        <v>0.008410101744404068</v>
       </c>
       <c r="H14" t="n">
         <v>0.009368558390742335</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.001431977625279105</v>
+        <v>-0.001428941817157672</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.008279181604903582</v>
+        <v>-0.008813954048211744</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.006607090920283636</v>
+        <v>-0.01652877714115108</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.006607090920283636</v>
+        <v>-0.01652877714115108</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.006607090920283636</v>
+        <v>-0.01652877714115108</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.006607090920283636</v>
+        <v>-0.01652877714115108</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.006607090920283636</v>
+        <v>-0.01652877714115108</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.008900467940018716</v>
+        <v>-0.01072841073313643</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.008446189201847566</v>
+        <v>-0.01452362534894501</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.008446189201847566</v>
+        <v>-0.01452362534894501</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.008446189201847566</v>
+        <v>-0.01452362534894501</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.008446189201847566</v>
+        <v>-0.01452362534894501</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.03756644886265795</v>
+        <v>-0.03758924924756997</v>
       </c>
       <c r="V14" t="n">
         <v>-0.01023091903323676</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.0009166274286650971</v>
+        <v>-0.0009165371886614874</v>
       </c>
       <c r="X14" t="n">
-        <v>-0.01037969110318764</v>
+        <v>-0.01038141353525654</v>
       </c>
       <c r="Y14" t="n">
         <v>0.01157249959889998</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.006962455574498222</v>
+        <v>-0.006703059436122376</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.01310771985230879</v>
+        <v>0.01856160976646439</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.01310771985230879</v>
+        <v>0.01856160976646439</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.01310771985230879</v>
+        <v>0.01856160976646439</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.01310771985230879</v>
+        <v>0.01856160976646439</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.01310771985230879</v>
+        <v>0.01856160976646439</v>
       </c>
     </row>
     <row r="15">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.001993477135739085</v>
+        <v>-0.001993553935742157</v>
       </c>
       <c r="D15" t="n">
         <v>-0.01063130442525218</v>
@@ -1819,79 +1819,79 @@
         <v>-0.01749456079578243</v>
       </c>
       <c r="G15" t="n">
-        <v>0.01710960606038424</v>
+        <v>0.01710964167638566</v>
       </c>
       <c r="H15" t="n">
         <v>0.01783614973744599</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.001191276623651065</v>
+        <v>-0.001189527887581115</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.01286916950590092</v>
+        <v>-0.01314648568520759</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.01117776889511076</v>
+        <v>0.004767438910697555</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.01117776889511076</v>
+        <v>0.004767438910697555</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.01117776889511076</v>
+        <v>0.004767438910697555</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.01117776889511076</v>
+        <v>0.004767438910697555</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.01117776889511076</v>
+        <v>0.004767438910697555</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.01724442673777707</v>
+        <v>-0.01573280530131221</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.01542077831283113</v>
+        <v>-0.006562304230492168</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.01542077831283113</v>
+        <v>-0.006562304230492168</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.01542077831283113</v>
+        <v>-0.006562304230492168</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.01542077831283113</v>
+        <v>-0.006562304230492168</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.02574890080595603</v>
+        <v>-0.02572778128511125</v>
       </c>
       <c r="V15" t="n">
         <v>-0.001893033675721347</v>
       </c>
       <c r="W15" t="n">
-        <v>0.008793528063741122</v>
+        <v>0.008792232351689291</v>
       </c>
       <c r="X15" t="n">
-        <v>-0.014705525004221</v>
+        <v>-0.01471183057247322</v>
       </c>
       <c r="Y15" t="n">
         <v>0.007909432060377282</v>
       </c>
       <c r="Z15" t="n">
-        <v>-0.01181248300049932</v>
+        <v>-0.01205289936211597</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.01518037721521509</v>
+        <v>0.0114661474346459</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.01518037721521509</v>
+        <v>0.0114661474346459</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.01518037721521509</v>
+        <v>0.0114661474346459</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.01518037721521509</v>
+        <v>0.0114661474346459</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.01518037721521509</v>
+        <v>0.0114661474346459</v>
       </c>
     </row>
     <row r="16">
@@ -1906,7 +1906,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.003750048726001949</v>
+        <v>0.003751480662059226</v>
       </c>
       <c r="D16" t="n">
         <v>0.01187364479494579</v>
@@ -1918,79 +1918,79 @@
         <v>-0.008066034850641394</v>
       </c>
       <c r="G16" t="n">
-        <v>0.01208644233945769</v>
+        <v>0.01208666582746663</v>
       </c>
       <c r="H16" t="n">
         <v>0.009797464039898561</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01324332446573298</v>
+        <v>0.01324164043366562</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.00103871236277002</v>
+        <v>-0.001244007219969645</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.006909416820376672</v>
+        <v>-0.0002724042348961693</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.006909416820376672</v>
+        <v>-0.0002724042348961693</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.006909416820376672</v>
+        <v>-0.0002724042348961693</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.006909416820376672</v>
+        <v>-0.0002724042348961693</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.006909416820376672</v>
+        <v>-0.0002724042348961693</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.009252537970101516</v>
+        <v>-0.00915008475000339</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.00402045078481803</v>
+        <v>-0.001715382404615296</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.00402045078481803</v>
+        <v>-0.001715382404615296</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.00402045078481803</v>
+        <v>-0.001715382404615296</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.00402045078481803</v>
+        <v>-0.001715382404615296</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.04008643158745726</v>
+        <v>-0.04008503200340128</v>
       </c>
       <c r="V16" t="n">
         <v>-0.02933400414936016</v>
       </c>
       <c r="W16" t="n">
-        <v>0.006825483729019349</v>
+        <v>0.006826271313050853</v>
       </c>
       <c r="X16" t="n">
-        <v>0.001264839122593565</v>
+        <v>0.001271202098848084</v>
       </c>
       <c r="Y16" t="n">
         <v>0.007160440990417639</v>
       </c>
       <c r="Z16" t="n">
-        <v>-0.0005341925973677039</v>
+        <v>-0.0005380143575205742</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.00778312427932497</v>
+        <v>0.007876128603045143</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.00778312427932497</v>
+        <v>0.007876128603045143</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.00778312427932497</v>
+        <v>0.007876128603045143</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.00778312427932497</v>
+        <v>0.007876128603045143</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.00778312427932497</v>
+        <v>0.007876128603045143</v>
       </c>
     </row>
     <row r="17">
@@ -2001,7 +2001,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.01555569019022761</v>
+        <v>0.01555436443017457</v>
       </c>
       <c r="D17" t="n">
         <v>-0.006570467302818691</v>
@@ -2013,79 +2013,79 @@
         <v>-0.01776617226264689</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01985300181812007</v>
+        <v>0.01985266447410658</v>
       </c>
       <c r="H17" t="n">
         <v>0.0160214951688598</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0005749068709962747</v>
+        <v>0.0005729134309165371</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.01489398315727465</v>
+        <v>-0.01432904915861036</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.02133091774923671</v>
+        <v>-0.007162327102493084</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.02133091774923671</v>
+        <v>-0.007162327102493084</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.02133091774923671</v>
+        <v>-0.007162327102493084</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.02133091774923671</v>
+        <v>-0.007162327102493084</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.02133091774923671</v>
+        <v>-0.007162327102493084</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.01914532406181296</v>
+        <v>-0.01941493460059738</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.0177067350122694</v>
+        <v>-0.01582453560898142</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.0177067350122694</v>
+        <v>-0.01582453560898142</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.0177067350122694</v>
+        <v>-0.01582453560898142</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.0177067350122694</v>
+        <v>-0.01582453560898142</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.007409144552365781</v>
+        <v>-0.007366160838646432</v>
       </c>
       <c r="V17" t="n">
         <v>-0.007322720740908829</v>
       </c>
       <c r="W17" t="n">
-        <v>0.008387337647493503</v>
+        <v>0.008387909039516361</v>
       </c>
       <c r="X17" t="n">
-        <v>-0.01393405063736202</v>
+        <v>-0.01393448446137938</v>
       </c>
       <c r="Y17" t="n">
         <v>-0.003868931290757251</v>
       </c>
       <c r="Z17" t="n">
-        <v>-0.01520184656007386</v>
+        <v>-0.01553385700535428</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.01990375289215011</v>
+        <v>0.01765530953821238</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.01990375289215011</v>
+        <v>0.01765530953821238</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.01990375289215011</v>
+        <v>0.01765530953821238</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.01990375289215011</v>
+        <v>0.01765530953821238</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.01990375289215011</v>
+        <v>0.01765530953821238</v>
       </c>
     </row>
     <row r="18">
@@ -2100,7 +2100,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.0158863174674527</v>
+        <v>-0.0158852399634096</v>
       </c>
       <c r="D18" t="n">
         <v>-0.004741255389650215</v>
@@ -2112,79 +2112,79 @@
         <v>0.004004380288175211</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.00403897878555915</v>
+        <v>-0.004039330337573213</v>
       </c>
       <c r="H18" t="n">
         <v>-0.005595411967816478</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.00771467176458687</v>
+        <v>-0.00768793105951724</v>
       </c>
       <c r="J18" t="n">
-        <v>0.01864240641561973</v>
+        <v>0.01946044996497976</v>
       </c>
       <c r="K18" t="n">
-        <v>0.005055156586206263</v>
+        <v>0.01456531911061276</v>
       </c>
       <c r="L18" t="n">
-        <v>0.005055156586206263</v>
+        <v>0.01456531911061276</v>
       </c>
       <c r="M18" t="n">
-        <v>0.005055156586206263</v>
+        <v>0.01456531911061276</v>
       </c>
       <c r="N18" t="n">
-        <v>0.005055156586206263</v>
+        <v>0.01456531911061276</v>
       </c>
       <c r="O18" t="n">
-        <v>0.005055156586206263</v>
+        <v>0.01456531911061276</v>
       </c>
       <c r="P18" t="n">
-        <v>0.003678910899156436</v>
+        <v>0.004953342822133712</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.006172579542903181</v>
+        <v>0.01196315385452615</v>
       </c>
       <c r="R18" t="n">
-        <v>0.006172579542903181</v>
+        <v>0.01196315385452615</v>
       </c>
       <c r="S18" t="n">
-        <v>0.006172579542903181</v>
+        <v>0.01196315385452615</v>
       </c>
       <c r="T18" t="n">
-        <v>0.006172579542903181</v>
+        <v>0.01196315385452615</v>
       </c>
       <c r="U18" t="n">
-        <v>0.01745687196227488</v>
+        <v>0.01741933384877335</v>
       </c>
       <c r="V18" t="n">
         <v>-0.01004119902564796</v>
       </c>
       <c r="W18" t="n">
-        <v>-0.01744695775387831</v>
+        <v>-0.01744644933785797</v>
       </c>
       <c r="X18" t="n">
-        <v>0.01407349995494</v>
+        <v>0.01407165176286607</v>
       </c>
       <c r="Y18" t="n">
         <v>-0.004277911275116451</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.01104346882573875</v>
+        <v>0.01139938730397549</v>
       </c>
       <c r="AA18" t="n">
-        <v>-0.01588082300323292</v>
+        <v>-0.01715317239812689</v>
       </c>
       <c r="AB18" t="n">
-        <v>-0.01588082300323292</v>
+        <v>-0.01715317239812689</v>
       </c>
       <c r="AC18" t="n">
-        <v>-0.01588082300323292</v>
+        <v>-0.01715317239812689</v>
       </c>
       <c r="AD18" t="n">
-        <v>-0.01588082300323292</v>
+        <v>-0.01715317239812689</v>
       </c>
       <c r="AE18" t="n">
-        <v>-0.01588082300323292</v>
+        <v>-0.01715317239812689</v>
       </c>
     </row>
     <row r="19">
@@ -2199,7 +2199,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.03902419231296769</v>
+        <v>-0.03901537576861503</v>
       </c>
       <c r="D19" t="n">
         <v>-0.005024797256991891</v>
@@ -2211,79 +2211,79 @@
         <v>0.01265202473008099</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.0121405323896213</v>
+        <v>-0.01214075952563038</v>
       </c>
       <c r="H19" t="n">
         <v>-0.01492228552489142</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.009978938031157519</v>
+        <v>-0.009990729903629194</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.003051885245664427</v>
+        <v>-0.003085726160909296</v>
       </c>
       <c r="K19" t="n">
-        <v>0.001523130108925204</v>
+        <v>0.002364115582564623</v>
       </c>
       <c r="L19" t="n">
-        <v>0.001523130108925204</v>
+        <v>0.002364115582564623</v>
       </c>
       <c r="M19" t="n">
-        <v>0.001523130108925204</v>
+        <v>0.002364115582564623</v>
       </c>
       <c r="N19" t="n">
-        <v>0.001523130108925204</v>
+        <v>0.002364115582564623</v>
       </c>
       <c r="O19" t="n">
-        <v>0.001523130108925204</v>
+        <v>0.002364115582564623</v>
       </c>
       <c r="P19" t="n">
-        <v>0.01223116215324649</v>
+        <v>0.01217429971897199</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.009895883531835341</v>
+        <v>0.009940928077637121</v>
       </c>
       <c r="R19" t="n">
-        <v>0.009895883531835341</v>
+        <v>0.009940928077637121</v>
       </c>
       <c r="S19" t="n">
-        <v>0.009895883531835341</v>
+        <v>0.009940928077637121</v>
       </c>
       <c r="T19" t="n">
-        <v>0.009895883531835341</v>
+        <v>0.009940928077637121</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.01805461790618471</v>
+        <v>-0.01807713038708521</v>
       </c>
       <c r="V19" t="n">
         <v>0.003903905244156209</v>
       </c>
       <c r="W19" t="n">
-        <v>0.01321573915262956</v>
+        <v>0.013216575120663</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.00937222904688916</v>
+        <v>-0.009373157558926301</v>
       </c>
       <c r="Y19" t="n">
         <v>-0.01330842302833692</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.009001196808047871</v>
+        <v>0.009239670609586822</v>
       </c>
       <c r="AA19" t="n">
-        <v>-0.00260467824818713</v>
+        <v>-0.004265832554633302</v>
       </c>
       <c r="AB19" t="n">
-        <v>-0.00260467824818713</v>
+        <v>-0.004265832554633302</v>
       </c>
       <c r="AC19" t="n">
-        <v>-0.00260467824818713</v>
+        <v>-0.004265832554633302</v>
       </c>
       <c r="AD19" t="n">
-        <v>-0.00260467824818713</v>
+        <v>-0.004265832554633302</v>
       </c>
       <c r="AE19" t="n">
-        <v>-0.00260467824818713</v>
+        <v>-0.004265832554633302</v>
       </c>
     </row>
     <row r="20">
@@ -2294,7 +2294,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.01921231689649268</v>
+        <v>0.01921528656061146</v>
       </c>
       <c r="D20" t="n">
         <v>-0.006169556118782244</v>
@@ -2306,79 +2306,79 @@
         <v>-0.008085116195404645</v>
       </c>
       <c r="G20" t="n">
-        <v>0.006297789275911571</v>
+        <v>0.00629765650790626</v>
       </c>
       <c r="H20" t="n">
         <v>0.006093610035744402</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.004491036179641447</v>
+        <v>-0.004497549491901979</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.007871707812125442</v>
+        <v>-0.007749426467740041</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.01575560607022424</v>
+        <v>-0.01235386129415445</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.01575560607022424</v>
+        <v>-0.01235386129415445</v>
       </c>
       <c r="M20" t="n">
-        <v>-0.01575560607022424</v>
+        <v>-0.01235386129415445</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.01575560607022424</v>
+        <v>-0.01235386129415445</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.01575560607022424</v>
+        <v>-0.01235386129415445</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.008259339498373578</v>
+        <v>-0.008751224702048987</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.01221480768859231</v>
+        <v>-0.01430575574023023</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.01221480768859231</v>
+        <v>-0.01430575574023023</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.01221480768859231</v>
+        <v>-0.01430575574023023</v>
       </c>
       <c r="T20" t="n">
-        <v>-0.01221480768859231</v>
+        <v>-0.01430575574023023</v>
       </c>
       <c r="U20" t="n">
-        <v>0.008405326416213055</v>
+        <v>0.008408029680321187</v>
       </c>
       <c r="V20" t="n">
         <v>0.02006072557042902</v>
       </c>
       <c r="W20" t="n">
-        <v>0.01471209879648395</v>
+        <v>0.01471122644444906</v>
       </c>
       <c r="X20" t="n">
-        <v>-0.008073287554931502</v>
+        <v>-0.008073972514958901</v>
       </c>
       <c r="Y20" t="n">
         <v>-0.0143706526068261</v>
       </c>
       <c r="Z20" t="n">
-        <v>-0.009345641749825669</v>
+        <v>-0.009376130295045212</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.002003901968156079</v>
+        <v>0.00454549477381979</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.002003901968156079</v>
+        <v>0.00454549477381979</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.002003901968156079</v>
+        <v>0.00454549477381979</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.002003901968156079</v>
+        <v>0.00454549477381979</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.002003901968156079</v>
+        <v>0.00454549477381979</v>
       </c>
     </row>
     <row r="21">
@@ -2389,7 +2389,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.004721057660842305</v>
+        <v>-0.004720993820839752</v>
       </c>
       <c r="D21" t="n">
         <v>-0.01017601365504055</v>
@@ -2401,79 +2401,79 @@
         <v>-0.01009437025977481</v>
       </c>
       <c r="G21" t="n">
-        <v>0.006099200595968023</v>
+        <v>0.00609907473996299</v>
       </c>
       <c r="H21" t="n">
         <v>0.005823191944927677</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.007054094586163782</v>
+        <v>-0.007058576634343064</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.006355925829711602</v>
+        <v>-0.005848743508337109</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.008336370669454826</v>
+        <v>-0.001305878356235134</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.008336370669454826</v>
+        <v>-0.001305878356235134</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.008336370669454826</v>
+        <v>-0.001305878356235134</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.008336370669454826</v>
+        <v>-0.001305878356235134</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.008336370669454826</v>
+        <v>-0.001305878356235134</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.009334688053387521</v>
+        <v>-0.009330513973220558</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.01224674295386972</v>
+        <v>-0.008331441165257645</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.01224674295386972</v>
+        <v>-0.008331441165257645</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.01224674295386972</v>
+        <v>-0.008331441165257645</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.01224674295386972</v>
+        <v>-0.008331441165257645</v>
       </c>
       <c r="U21" t="n">
-        <v>-0.0005538862301554491</v>
+        <v>-0.0005601513824060552</v>
       </c>
       <c r="V21" t="n">
         <v>0.01849270422770817</v>
       </c>
       <c r="W21" t="n">
-        <v>0.004230028297201131</v>
+        <v>0.004230826921233077</v>
       </c>
       <c r="X21" t="n">
-        <v>-0.0005517252700690106</v>
+        <v>-0.0005463783578551342</v>
       </c>
       <c r="Y21" t="n">
         <v>-0.01805642606625704</v>
       </c>
       <c r="Z21" t="n">
-        <v>-0.006227350329094012</v>
+        <v>-0.006203197208127887</v>
       </c>
       <c r="AA21" t="n">
-        <v>-0.009484015867360633</v>
+        <v>-0.008166038150641526</v>
       </c>
       <c r="AB21" t="n">
-        <v>-0.009484015867360633</v>
+        <v>-0.008166038150641526</v>
       </c>
       <c r="AC21" t="n">
-        <v>-0.009484015867360633</v>
+        <v>-0.008166038150641526</v>
       </c>
       <c r="AD21" t="n">
-        <v>-0.009484015867360633</v>
+        <v>-0.008166038150641526</v>
       </c>
       <c r="AE21" t="n">
-        <v>-0.009484015867360633</v>
+        <v>-0.008166038150641526</v>
       </c>
     </row>
     <row r="22">
@@ -2484,7 +2484,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.0004710826748433069</v>
+        <v>-0.0004620861304834452</v>
       </c>
       <c r="D22" t="n">
         <v>-0.01713025143721005</v>
@@ -2496,79 +2496,79 @@
         <v>0.02719278204771128</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.02745097127403885</v>
+        <v>-0.02745089130603565</v>
       </c>
       <c r="H22" t="n">
         <v>-0.02460165324006613</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.02881865712074628</v>
+        <v>-0.02880754780830191</v>
       </c>
       <c r="J22" t="n">
-        <v>0.03631391544726179</v>
+        <v>0.03656593155957836</v>
       </c>
       <c r="K22" t="n">
-        <v>0.02553978534159141</v>
+        <v>-0.001216328688653147</v>
       </c>
       <c r="L22" t="n">
-        <v>0.02553978534159141</v>
+        <v>-0.001216328688653147</v>
       </c>
       <c r="M22" t="n">
-        <v>0.02553978534159141</v>
+        <v>-0.001216328688653147</v>
       </c>
       <c r="N22" t="n">
-        <v>0.02553978534159141</v>
+        <v>-0.001216328688653147</v>
       </c>
       <c r="O22" t="n">
-        <v>0.02553978534159141</v>
+        <v>-0.001216328688653147</v>
       </c>
       <c r="P22" t="n">
-        <v>0.02797645619105824</v>
+        <v>0.02680692040027681</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.02742298573691943</v>
+        <v>0.01735375058215002</v>
       </c>
       <c r="R22" t="n">
-        <v>0.02742298573691943</v>
+        <v>0.01735375058215002</v>
       </c>
       <c r="S22" t="n">
-        <v>0.02742298573691943</v>
+        <v>0.01735375058215002</v>
       </c>
       <c r="T22" t="n">
-        <v>0.02742298573691943</v>
+        <v>0.01735375058215002</v>
       </c>
       <c r="U22" t="n">
-        <v>0.01548820410752816</v>
+        <v>0.01550238974009559</v>
       </c>
       <c r="V22" t="n">
         <v>0.001543964989758599</v>
       </c>
       <c r="W22" t="n">
-        <v>7.10659228426369e-06</v>
+        <v>7.558272302330892e-06</v>
       </c>
       <c r="X22" t="n">
-        <v>0.0272129125765165</v>
+        <v>0.02721392921655717</v>
       </c>
       <c r="Y22" t="n">
         <v>0.009851964586078583</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.01629847169193887</v>
+        <v>0.01621262714450509</v>
       </c>
       <c r="AA22" t="n">
-        <v>-0.03262560936902437</v>
+        <v>-0.02661750548070022</v>
       </c>
       <c r="AB22" t="n">
-        <v>-0.03262560936902437</v>
+        <v>-0.02661750548070022</v>
       </c>
       <c r="AC22" t="n">
-        <v>-0.03262560936902437</v>
+        <v>-0.02661750548070022</v>
       </c>
       <c r="AD22" t="n">
-        <v>-0.03262560936902437</v>
+        <v>-0.02661750548070022</v>
       </c>
       <c r="AE22" t="n">
-        <v>-0.03262560936902437</v>
+        <v>-0.02661750548070022</v>
       </c>
     </row>
     <row r="23">
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.01605421869016875</v>
+        <v>-0.01605513933020557</v>
       </c>
       <c r="D23" t="n">
         <v>-0.01255258629410345</v>
@@ -2595,79 +2595,79 @@
         <v>0.01285939654637586</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.01157817665512706</v>
+        <v>-0.01157838843113554</v>
       </c>
       <c r="H23" t="n">
         <v>-0.009545882301835291</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.01381992112879684</v>
+        <v>-0.01380220058408802</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0191935302943128</v>
+        <v>0.01965915912528103</v>
       </c>
       <c r="K23" t="n">
-        <v>0.02751207450848298</v>
+        <v>0.01589599215583968</v>
       </c>
       <c r="L23" t="n">
-        <v>0.02751207450848298</v>
+        <v>0.01589599215583968</v>
       </c>
       <c r="M23" t="n">
-        <v>0.02751207450848298</v>
+        <v>0.01589599215583968</v>
       </c>
       <c r="N23" t="n">
-        <v>0.02751207450848298</v>
+        <v>0.01589599215583968</v>
       </c>
       <c r="O23" t="n">
-        <v>0.02751207450848298</v>
+        <v>0.01589599215583968</v>
       </c>
       <c r="P23" t="n">
-        <v>0.01366750931470037</v>
+        <v>0.01365532941021317</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.02003128793725151</v>
+        <v>0.0198591050183642</v>
       </c>
       <c r="R23" t="n">
-        <v>0.02003128793725151</v>
+        <v>0.0198591050183642</v>
       </c>
       <c r="S23" t="n">
-        <v>0.02003128793725151</v>
+        <v>0.0198591050183642</v>
       </c>
       <c r="T23" t="n">
-        <v>0.02003128793725151</v>
+        <v>0.0198591050183642</v>
       </c>
       <c r="U23" t="n">
-        <v>-0.0009280328051213121</v>
+        <v>-0.0008825981153039245</v>
       </c>
       <c r="V23" t="n">
         <v>-0.01932179078887163</v>
       </c>
       <c r="W23" t="n">
-        <v>0.01362984544119382</v>
+        <v>0.01363028598521144</v>
       </c>
       <c r="X23" t="n">
-        <v>0.03924992576199703</v>
+        <v>0.03924327305773091</v>
       </c>
       <c r="Y23" t="n">
         <v>0.01562144059285762</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.02250230048409202</v>
+        <v>0.02203982814559312</v>
       </c>
       <c r="AA23" t="n">
-        <v>-0.02383495400939815</v>
+        <v>-0.02638470335938813</v>
       </c>
       <c r="AB23" t="n">
-        <v>-0.02383495400939815</v>
+        <v>-0.02638470335938813</v>
       </c>
       <c r="AC23" t="n">
-        <v>-0.02383495400939815</v>
+        <v>-0.02638470335938813</v>
       </c>
       <c r="AD23" t="n">
-        <v>-0.02383495400939815</v>
+        <v>-0.02638470335938813</v>
       </c>
       <c r="AE23" t="n">
-        <v>-0.02383495400939815</v>
+        <v>-0.02638470335938813</v>
       </c>
     </row>
     <row r="24">
@@ -2678,7 +2678,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.01895662981426519</v>
+        <v>0.01893625554145022</v>
       </c>
       <c r="D24" t="n">
         <v>0.02253726483749059</v>
@@ -2690,79 +2690,79 @@
         <v>0.0008928255717130228</v>
       </c>
       <c r="G24" t="n">
-        <v>0.001118957900758316</v>
+        <v>0.001118734028749361</v>
       </c>
       <c r="H24" t="n">
         <v>9.757075590283023e-05</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02053363445334537</v>
+        <v>0.02053750805350032</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0001155655247585261</v>
+        <v>8.724614764479506e-05</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0001314101812564072</v>
+        <v>-0.0203716376148655</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0001314101812564072</v>
+        <v>-0.0203716376148655</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0001314101812564072</v>
+        <v>-0.0203716376148655</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0001314101812564072</v>
+        <v>-0.0203716376148655</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0001314101812564072</v>
+        <v>-0.0203716376148655</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.0003198699967947998</v>
+        <v>-0.002087733395509335</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.001084060651362426</v>
+        <v>-0.01131082701243308</v>
       </c>
       <c r="R24" t="n">
-        <v>0.001084060651362426</v>
+        <v>-0.01131082701243308</v>
       </c>
       <c r="S24" t="n">
-        <v>0.001084060651362426</v>
+        <v>-0.01131082701243308</v>
       </c>
       <c r="T24" t="n">
-        <v>0.001084060651362426</v>
+        <v>-0.01131082701243308</v>
       </c>
       <c r="U24" t="n">
-        <v>0.0191263025250521</v>
+        <v>0.01910384418815377</v>
       </c>
       <c r="V24" t="n">
         <v>-0.009297761939910477</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.01430677055627082</v>
+        <v>-0.01430713535628541</v>
       </c>
       <c r="X24" t="n">
-        <v>-0.01306932474677299</v>
+        <v>-0.01306615914664636</v>
       </c>
       <c r="Y24" t="n">
         <v>0.01663220111328804</v>
       </c>
       <c r="Z24" t="n">
-        <v>-0.00331116925244677</v>
+        <v>-0.003095924571836982</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.01454205446968218</v>
+        <v>0.01755180300607212</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.01454205446968218</v>
+        <v>0.01755180300607212</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.01454205446968218</v>
+        <v>0.01755180300607212</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.01454205446968218</v>
+        <v>0.01755180300607212</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.01454205446968218</v>
+        <v>0.01755180300607212</v>
       </c>
     </row>
     <row r="25">
@@ -2777,7 +2777,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.0009693556227742249</v>
+        <v>-0.0009798170311926813</v>
       </c>
       <c r="D25" t="n">
         <v>0.0109187299727492</v>
@@ -2789,79 +2789,79 @@
         <v>0.01064734852189394</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.009249688113987523</v>
+        <v>-0.009249494001979759</v>
       </c>
       <c r="H25" t="n">
         <v>-0.01109573881182955</v>
       </c>
       <c r="I25" t="n">
-        <v>0.009777679207107167</v>
+        <v>0.009771261510850459</v>
       </c>
       <c r="J25" t="n">
-        <v>0.001524106910756626</v>
+        <v>0.001497769550570821</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.002911776020471041</v>
+        <v>0.01430948850837954</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.002911776020471041</v>
+        <v>0.01430948850837954</v>
       </c>
       <c r="M25" t="n">
-        <v>-0.002911776020471041</v>
+        <v>0.01430948850837954</v>
       </c>
       <c r="N25" t="n">
-        <v>-0.002911776020471041</v>
+        <v>0.01430948850837954</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.002911776020471041</v>
+        <v>0.01430948850837954</v>
       </c>
       <c r="P25" t="n">
-        <v>0.009553337470133497</v>
+        <v>0.01120602544024102</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.006879821171192846</v>
+        <v>0.0115335175493407</v>
       </c>
       <c r="R25" t="n">
-        <v>0.006879821171192846</v>
+        <v>0.0115335175493407</v>
       </c>
       <c r="S25" t="n">
-        <v>0.006879821171192846</v>
+        <v>0.0115335175493407</v>
       </c>
       <c r="T25" t="n">
-        <v>0.006879821171192846</v>
+        <v>0.0115335175493407</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.03447922899516916</v>
+        <v>-0.03449650889986035</v>
       </c>
       <c r="V25" t="n">
         <v>0.009190432111617283</v>
       </c>
       <c r="W25" t="n">
-        <v>-0.01034234460569378</v>
+        <v>-0.01034250233370009</v>
       </c>
       <c r="X25" t="n">
-        <v>-0.01818730114349204</v>
+        <v>-0.01818523935140957</v>
       </c>
       <c r="Y25" t="n">
         <v>-0.002636931945477277</v>
       </c>
       <c r="Z25" t="n">
-        <v>-0.01741656991266279</v>
+        <v>-0.01726288062651522</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.01413732968549319</v>
+        <v>0.008571740598869624</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.01413732968549319</v>
+        <v>0.008571740598869624</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.01413732968549319</v>
+        <v>0.008571740598869624</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.01413732968549319</v>
+        <v>0.008571740598869624</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.01413732968549319</v>
+        <v>0.008571740598869624</v>
       </c>
     </row>
     <row r="26">
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-0.009846384489855378</v>
+        <v>-0.009845103849804153</v>
       </c>
       <c r="D26" t="n">
         <v>-0.01001658673666347</v>
@@ -2884,79 +2884,79 @@
         <v>0.0004467351538694061</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.001768032454721298</v>
+        <v>-0.001768045990721839</v>
       </c>
       <c r="H26" t="n">
         <v>-0.001747847973913919</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.005966033134641325</v>
+        <v>-0.005984720495388818</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.01997378165444043</v>
+        <v>-0.02100186630137396</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.003470411370816454</v>
+        <v>-0.01639973326398933</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.003470411370816454</v>
+        <v>-0.01639973326398933</v>
       </c>
       <c r="M26" t="n">
-        <v>-0.003470411370816454</v>
+        <v>-0.01639973326398933</v>
       </c>
       <c r="N26" t="n">
-        <v>-0.003470411370816454</v>
+        <v>-0.01639973326398933</v>
       </c>
       <c r="O26" t="n">
-        <v>-0.003470411370816454</v>
+        <v>-0.01639973326398933</v>
       </c>
       <c r="P26" t="n">
-        <v>0.0009317985972719438</v>
+        <v>-0.0003986222559448901</v>
       </c>
       <c r="Q26" t="n">
-        <v>-0.001829682121187284</v>
+        <v>-0.01303031735321269</v>
       </c>
       <c r="R26" t="n">
-        <v>-0.001829682121187284</v>
+        <v>-0.01303031735321269</v>
       </c>
       <c r="S26" t="n">
-        <v>-0.001829682121187284</v>
+        <v>-0.01303031735321269</v>
       </c>
       <c r="T26" t="n">
-        <v>-0.001829682121187284</v>
+        <v>-0.01303031735321269</v>
       </c>
       <c r="U26" t="n">
-        <v>0.001324413940976558</v>
+        <v>0.00129716299588652</v>
       </c>
       <c r="V26" t="n">
         <v>0.01025919141836766</v>
       </c>
       <c r="W26" t="n">
-        <v>-0.02378156399126256</v>
+        <v>-0.02378240043929601</v>
       </c>
       <c r="X26" t="n">
-        <v>-0.0004322384812895391</v>
+        <v>-0.0004329139373165574</v>
       </c>
       <c r="Y26" t="n">
         <v>-0.006328827421153095</v>
       </c>
       <c r="Z26" t="n">
-        <v>-0.005280973747238949</v>
+        <v>-0.005056865674274626</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.0005688060707522428</v>
+        <v>0.00602935051317402</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.0005688060707522428</v>
+        <v>0.00602935051317402</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.0005688060707522428</v>
+        <v>0.00602935051317402</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.0005688060707522428</v>
+        <v>0.00602935051317402</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.0005688060707522428</v>
+        <v>0.00602935051317402</v>
       </c>
     </row>
     <row r="27">
@@ -2971,7 +2971,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-0.02352763207710528</v>
+        <v>-0.02351559358062374</v>
       </c>
       <c r="D27" t="n">
         <v>0.01890344744413789</v>
@@ -2983,79 +2983,79 @@
         <v>0.003793820215752808</v>
       </c>
       <c r="G27" t="n">
-        <v>0.02141376930455077</v>
+        <v>0.02141374194454967</v>
       </c>
       <c r="H27" t="n">
         <v>-0.005762388422495537</v>
       </c>
       <c r="I27" t="n">
-        <v>0.02913977578959103</v>
+        <v>0.02912930410917216</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.00829240066144789</v>
+        <v>-0.008419694463741157</v>
       </c>
       <c r="K27" t="n">
-        <v>0.05045403878616154</v>
+        <v>0.04377685634307425</v>
       </c>
       <c r="L27" t="n">
-        <v>0.05045403878616154</v>
+        <v>0.04377685634307425</v>
       </c>
       <c r="M27" t="n">
-        <v>0.05045403878616154</v>
+        <v>0.04377685634307425</v>
       </c>
       <c r="N27" t="n">
-        <v>0.05045403878616154</v>
+        <v>0.04377685634307425</v>
       </c>
       <c r="O27" t="n">
-        <v>0.05045403878616154</v>
+        <v>0.04377685634307425</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.002821333168853326</v>
+        <v>-0.0006929975317199013</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.04154618134184725</v>
+        <v>0.04854795938191837</v>
       </c>
       <c r="R27" t="n">
-        <v>0.04154618134184725</v>
+        <v>0.04854795938191837</v>
       </c>
       <c r="S27" t="n">
-        <v>0.04154618134184725</v>
+        <v>0.04854795938191837</v>
       </c>
       <c r="T27" t="n">
-        <v>0.04154618134184725</v>
+        <v>0.04854795938191837</v>
       </c>
       <c r="U27" t="n">
-        <v>-0.04688276894731075</v>
+        <v>-0.0468679151547166</v>
       </c>
       <c r="V27" t="n">
         <v>-0.2407262669090507</v>
       </c>
       <c r="W27" t="n">
-        <v>0.9916528404661135</v>
+        <v>0.9916527858421114</v>
       </c>
       <c r="X27" t="n">
-        <v>0.03827839708313589</v>
+        <v>0.03827723125908924</v>
       </c>
       <c r="Y27" t="n">
         <v>-0.06436975764679029</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.02942821644112865</v>
+        <v>0.02935049311001972</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.01710637335625493</v>
+        <v>0.004620073720802948</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.01710637335625493</v>
+        <v>0.004620073720802948</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.01710637335625493</v>
+        <v>0.004620073720802948</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.01710637335625493</v>
+        <v>0.004620073720802948</v>
       </c>
       <c r="AE27" t="n">
-        <v>0.01710637335625493</v>
+        <v>0.004620073720802948</v>
       </c>
     </row>
     <row r="28">
@@ -3070,7 +3070,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.006993071511722859</v>
+        <v>-0.007008992728359709</v>
       </c>
       <c r="D28" t="n">
         <v>-0.008152086854083472</v>
@@ -3082,79 +3082,79 @@
         <v>0.001561438046457521</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0002037729681509187</v>
+        <v>0.0002038813521552541</v>
       </c>
       <c r="H28" t="n">
         <v>0.001382082199283288</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.007828105561124222</v>
+        <v>-0.007819993752799749</v>
       </c>
       <c r="J28" t="n">
-        <v>0.009853224645716379</v>
+        <v>0.00880146617569005</v>
       </c>
       <c r="K28" t="n">
-        <v>0.001907634988305399</v>
+        <v>0.01404666766586671</v>
       </c>
       <c r="L28" t="n">
-        <v>0.001907634988305399</v>
+        <v>0.01404666766586671</v>
       </c>
       <c r="M28" t="n">
-        <v>0.001907634988305399</v>
+        <v>0.01404666766586671</v>
       </c>
       <c r="N28" t="n">
-        <v>0.001907634988305399</v>
+        <v>0.01404666766586671</v>
       </c>
       <c r="O28" t="n">
-        <v>0.001907634988305399</v>
+        <v>0.01404666766586671</v>
       </c>
       <c r="P28" t="n">
-        <v>0.001615352896614115</v>
+        <v>0.002977141655085665</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.003562341742493669</v>
+        <v>0.009542341149693646</v>
       </c>
       <c r="R28" t="n">
-        <v>0.003562341742493669</v>
+        <v>0.009542341149693646</v>
       </c>
       <c r="S28" t="n">
-        <v>0.003562341742493669</v>
+        <v>0.009542341149693646</v>
       </c>
       <c r="T28" t="n">
-        <v>0.003562341742493669</v>
+        <v>0.009542341149693646</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.004741650909666036</v>
+        <v>-0.004791684959667398</v>
       </c>
       <c r="V28" t="n">
         <v>-0.01035864579034583</v>
       </c>
       <c r="W28" t="n">
-        <v>0.01207957661118306</v>
+        <v>0.01207927209917088</v>
       </c>
       <c r="X28" t="n">
-        <v>0.004745535357821414</v>
+        <v>0.00474211900568476</v>
       </c>
       <c r="Y28" t="n">
         <v>0.01080725457629018</v>
       </c>
       <c r="Z28" t="n">
-        <v>-0.001915044652601786</v>
+        <v>-0.001441282329651293</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.003794505847780233</v>
+        <v>0.0004809581952383278</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.003794505847780233</v>
+        <v>0.0004809581952383278</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.003794505847780233</v>
+        <v>0.0004809581952383278</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.003794505847780233</v>
+        <v>0.0004809581952383278</v>
       </c>
       <c r="AE28" t="n">
-        <v>0.003794505847780233</v>
+        <v>0.0004809581952383278</v>
       </c>
     </row>
     <row r="29">
@@ -3169,7 +3169,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.009210923888436954</v>
+        <v>0.009217309136692364</v>
       </c>
       <c r="D29" t="n">
         <v>0.01661224492048979</v>
@@ -3181,79 +3181,79 @@
         <v>-0.02176001789440071</v>
       </c>
       <c r="G29" t="n">
-        <v>0.02500894967235798</v>
+        <v>0.02500891636035665</v>
       </c>
       <c r="H29" t="n">
         <v>0.02448300213132008</v>
       </c>
       <c r="I29" t="n">
-        <v>0.02611430677257227</v>
+        <v>0.02606282177851287</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.08442504808428578</v>
+        <v>-0.08420289294166006</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.003983923071356922</v>
+        <v>0.02220227196009087</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.003983923071356922</v>
+        <v>0.02220227196009087</v>
       </c>
       <c r="M29" t="n">
-        <v>-0.003983923071356922</v>
+        <v>0.02220227196009087</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.003983923071356922</v>
+        <v>0.02220227196009087</v>
       </c>
       <c r="O29" t="n">
-        <v>-0.003983923071356922</v>
+        <v>0.02220227196009087</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.02260037783201511</v>
+        <v>-0.01962733672109346</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.01874837316593492</v>
+        <v>-0.002892370483694819</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.01874837316593492</v>
+        <v>-0.002892370483694819</v>
       </c>
       <c r="S29" t="n">
-        <v>-0.01874837316593492</v>
+        <v>-0.002892370483694819</v>
       </c>
       <c r="T29" t="n">
-        <v>-0.01874837316593492</v>
+        <v>-0.002892370483694819</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.01544812890592515</v>
+        <v>-0.01548121636324865</v>
       </c>
       <c r="V29" t="n">
         <v>0.01274973804598952</v>
       </c>
       <c r="W29" t="n">
-        <v>0.1306126068885043</v>
+        <v>0.1306130205525208</v>
       </c>
       <c r="X29" t="n">
-        <v>-0.03289818553992741</v>
+        <v>-0.03289998285199931</v>
       </c>
       <c r="Y29" t="n">
         <v>0.007299384579975382</v>
       </c>
       <c r="Z29" t="n">
-        <v>-0.01355772121430884</v>
+        <v>-0.01325905099436204</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.04425503389820135</v>
+        <v>0.03186129314645172</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.04425503389820135</v>
+        <v>0.03186129314645172</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.04425503389820135</v>
+        <v>0.03186129314645172</v>
       </c>
       <c r="AD29" t="n">
-        <v>0.04425503389820135</v>
+        <v>0.03186129314645172</v>
       </c>
       <c r="AE29" t="n">
-        <v>0.04425503389820135</v>
+        <v>0.03186129314645172</v>
       </c>
     </row>
     <row r="30">
@@ -3268,7 +3268,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.005295288595811544</v>
+        <v>-0.005307454964298198</v>
       </c>
       <c r="D30" t="n">
         <v>-0.01542497485699899</v>
@@ -3280,79 +3280,79 @@
         <v>0.002351465662058626</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.001895791947831677</v>
+        <v>-0.001895809323832373</v>
       </c>
       <c r="H30" t="n">
         <v>-0.0007095833563833342</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.01932901344516054</v>
+        <v>-0.01930139914005597</v>
       </c>
       <c r="J30" t="n">
-        <v>0.01562003281917047</v>
+        <v>0.01577898449918286</v>
       </c>
       <c r="K30" t="n">
-        <v>0.01236940523077621</v>
+        <v>0.02049292661171706</v>
       </c>
       <c r="L30" t="n">
-        <v>0.01236940523077621</v>
+        <v>0.02049292661171706</v>
       </c>
       <c r="M30" t="n">
-        <v>0.01236940523077621</v>
+        <v>0.02049292661171706</v>
       </c>
       <c r="N30" t="n">
-        <v>0.01236940523077621</v>
+        <v>0.02049292661171706</v>
       </c>
       <c r="O30" t="n">
-        <v>0.01236940523077621</v>
+        <v>0.02049292661171706</v>
       </c>
       <c r="P30" t="n">
-        <v>0.003094344987773799</v>
+        <v>0.004941311717652468</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.008977564295102571</v>
+        <v>0.01370144291605772</v>
       </c>
       <c r="R30" t="n">
-        <v>0.008977564295102571</v>
+        <v>0.01370144291605772</v>
       </c>
       <c r="S30" t="n">
-        <v>0.008977564295102571</v>
+        <v>0.01370144291605772</v>
       </c>
       <c r="T30" t="n">
-        <v>0.008977564295102571</v>
+        <v>0.01370144291605772</v>
       </c>
       <c r="U30" t="n">
-        <v>0.02467647737105909</v>
+        <v>0.02470655906826236</v>
       </c>
       <c r="V30" t="n">
         <v>-0.0217936400717456</v>
       </c>
       <c r="W30" t="n">
-        <v>-0.01281354876854195</v>
+        <v>-0.01281493990459759</v>
       </c>
       <c r="X30" t="n">
-        <v>0.02996840366273614</v>
+        <v>0.02996553076662123</v>
       </c>
       <c r="Y30" t="n">
         <v>0.008859451746378068</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.01331131205245248</v>
+        <v>0.01311404826856193</v>
       </c>
       <c r="AA30" t="n">
-        <v>-0.02019344432773777</v>
+        <v>-0.02559472460778898</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.02019344432773777</v>
+        <v>-0.02559472460778898</v>
       </c>
       <c r="AC30" t="n">
-        <v>-0.02019344432773777</v>
+        <v>-0.02559472460778898</v>
       </c>
       <c r="AD30" t="n">
-        <v>-0.02019344432773777</v>
+        <v>-0.02559472460778898</v>
       </c>
       <c r="AE30" t="n">
-        <v>-0.02019344432773777</v>
+        <v>-0.02559472460778898</v>
       </c>
     </row>
     <row r="31">
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.4973775108711004</v>
+        <v>0.4973303725652148</v>
       </c>
       <c r="D31" t="n">
         <v>-0.02025557121022284</v>
@@ -3379,79 +3379,79 @@
         <v>-0.9999571538542861</v>
       </c>
       <c r="G31" t="n">
-        <v>0.9915449942537996</v>
+        <v>0.9915449903177994</v>
       </c>
       <c r="H31" t="n">
         <v>0.986521855012874</v>
       </c>
       <c r="I31" t="n">
-        <v>0.3790229966329198</v>
+        <v>0.3790263997370559</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.5043761605281928</v>
+        <v>-0.5044739135069023</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.79655625119025</v>
+        <v>-0.3014652584266103</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.79655625119025</v>
+        <v>-0.3014652584266103</v>
       </c>
       <c r="M31" t="n">
-        <v>-0.79655625119025</v>
+        <v>-0.3014652584266103</v>
       </c>
       <c r="N31" t="n">
-        <v>-0.79655625119025</v>
+        <v>-0.3014652584266103</v>
       </c>
       <c r="O31" t="n">
-        <v>-0.79655625119025</v>
+        <v>-0.3014652584266103</v>
       </c>
       <c r="P31" t="n">
-        <v>-0.9988880891715235</v>
+        <v>-0.994245954553838</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.9605882159275285</v>
+        <v>-0.808925152805006</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.9605882159275285</v>
+        <v>-0.808925152805006</v>
       </c>
       <c r="S31" t="n">
-        <v>-0.9605882159275285</v>
+        <v>-0.808925152805006</v>
       </c>
       <c r="T31" t="n">
-        <v>-0.9605882159275285</v>
+        <v>-0.808925152805006</v>
       </c>
       <c r="U31" t="n">
-        <v>-0.1280950321318013</v>
+        <v>-0.1281064438442577</v>
       </c>
       <c r="V31" t="n">
         <v>-0.005516132956645317</v>
       </c>
       <c r="W31" t="n">
-        <v>0.006118446580737862</v>
+        <v>0.006118873492754938</v>
       </c>
       <c r="X31" t="n">
-        <v>-0.4121343537333741</v>
+        <v>-0.4121335171893407</v>
       </c>
       <c r="Y31" t="n">
         <v>0.004067990850719633</v>
       </c>
       <c r="Z31" t="n">
-        <v>-0.4864116549764661</v>
+        <v>-0.48640125232005</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.5272385632015424</v>
+        <v>0.5065029048041161</v>
       </c>
       <c r="AB31" t="n">
-        <v>0.5272385632015424</v>
+        <v>0.5065029048041161</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.5272385632015424</v>
+        <v>0.5065029048041161</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.5272385632015424</v>
+        <v>0.5065029048041161</v>
       </c>
       <c r="AE31" t="n">
-        <v>0.5272385632015424</v>
+        <v>0.5065029048041161</v>
       </c>
     </row>
     <row r="32">
@@ -3466,7 +3466,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.003744595445783817</v>
+        <v>0.003748434101937363</v>
       </c>
       <c r="D32" t="n">
         <v>-0.01117334454293378</v>
@@ -3478,79 +3478,79 @@
         <v>-0.02709254642770185</v>
       </c>
       <c r="G32" t="n">
-        <v>0.02444281086571243</v>
+        <v>0.02444242331369693</v>
       </c>
       <c r="H32" t="n">
         <v>0.02768605598744224</v>
       </c>
       <c r="I32" t="n">
-        <v>0.001215286704611468</v>
+        <v>0.001222073712882948</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.002818072052036935</v>
+        <v>-0.002411816308756038</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.02421549792861992</v>
+        <v>-0.002058335602333424</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.02421549792861992</v>
+        <v>-0.002058335602333424</v>
       </c>
       <c r="M32" t="n">
-        <v>-0.02421549792861992</v>
+        <v>-0.002058335602333424</v>
       </c>
       <c r="N32" t="n">
-        <v>-0.02421549792861992</v>
+        <v>-0.002058335602333424</v>
       </c>
       <c r="O32" t="n">
-        <v>-0.02421549792861992</v>
+        <v>-0.002058335602333424</v>
       </c>
       <c r="P32" t="n">
-        <v>-0.02591999796479991</v>
+        <v>-0.02482273884890955</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.02795937471837498</v>
+        <v>-0.02088803718752149</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.02795937471837498</v>
+        <v>-0.02088803718752149</v>
       </c>
       <c r="S32" t="n">
-        <v>-0.02795937471837498</v>
+        <v>-0.02088803718752149</v>
       </c>
       <c r="T32" t="n">
-        <v>-0.02795937471837498</v>
+        <v>-0.02088803718752149</v>
       </c>
       <c r="U32" t="n">
-        <v>-0.01254051957362078</v>
+        <v>-0.01253932053357282</v>
       </c>
       <c r="V32" t="n">
         <v>0.006739304237572169</v>
       </c>
       <c r="W32" t="n">
-        <v>0.00440712152028486</v>
+        <v>0.004407681200307247</v>
       </c>
       <c r="X32" t="n">
-        <v>-0.001191004655640186</v>
+        <v>-0.001190355887614235</v>
       </c>
       <c r="Y32" t="n">
         <v>0.001241462737658509</v>
       </c>
       <c r="Z32" t="n">
-        <v>-0.007457047018281879</v>
+        <v>-0.007472142154885684</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.00323660825746433</v>
+        <v>0.001720714724828589</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.00323660825746433</v>
+        <v>0.001720714724828589</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.00323660825746433</v>
+        <v>0.001720714724828589</v>
       </c>
       <c r="AD32" t="n">
-        <v>0.00323660825746433</v>
+        <v>0.001720714724828589</v>
       </c>
       <c r="AE32" t="n">
-        <v>0.00323660825746433</v>
+        <v>0.001720714724828589</v>
       </c>
     </row>
     <row r="33">
@@ -3565,7 +3565,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.03210589568423582</v>
+        <v>-0.03211283168451327</v>
       </c>
       <c r="D33" t="n">
         <v>-0.001813062024522481</v>
@@ -3577,79 +3577,79 @@
         <v>-0.02417522631100905</v>
       </c>
       <c r="G33" t="n">
-        <v>0.02399404627176185</v>
+        <v>0.02399428684777147</v>
       </c>
       <c r="H33" t="n">
         <v>0.02335090048603602</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01468599073143963</v>
+        <v>0.01468776874751075</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.0585770448599684</v>
+        <v>-0.0590261488498764</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0167171301086852</v>
+        <v>0.004146969381878775</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0167171301086852</v>
+        <v>0.004146969381878775</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0167171301086852</v>
+        <v>0.004146969381878775</v>
       </c>
       <c r="N33" t="n">
-        <v>0.0167171301086852</v>
+        <v>0.004146969381878775</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0167171301086852</v>
+        <v>0.004146969381878775</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.02280676056027042</v>
+        <v>-0.02365378318615132</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.0106609376104375</v>
+        <v>-0.01162267659290706</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.0106609376104375</v>
+        <v>-0.01162267659290706</v>
       </c>
       <c r="S33" t="n">
-        <v>-0.0106609376104375</v>
+        <v>-0.01162267659290706</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.0106609376104375</v>
+        <v>-0.01162267659290706</v>
       </c>
       <c r="U33" t="n">
-        <v>-0.02320236582409463</v>
+        <v>-0.02318750454350018</v>
       </c>
       <c r="V33" t="n">
         <v>-0.01567911029116441</v>
       </c>
       <c r="W33" t="n">
-        <v>0.02237992995119719</v>
+        <v>0.02238013942320557</v>
       </c>
       <c r="X33" t="n">
-        <v>-0.01699915411996616</v>
+        <v>-0.01699841626393665</v>
       </c>
       <c r="Y33" t="n">
         <v>0.0006461822658472905</v>
       </c>
       <c r="Z33" t="n">
-        <v>-0.0201530024061201</v>
+        <v>-0.02027913306716532</v>
       </c>
       <c r="AA33" t="n">
-        <v>0.03900982591239303</v>
+        <v>0.03353416050936642</v>
       </c>
       <c r="AB33" t="n">
-        <v>0.03900982591239303</v>
+        <v>0.03353416050936642</v>
       </c>
       <c r="AC33" t="n">
-        <v>0.03900982591239303</v>
+        <v>0.03353416050936642</v>
       </c>
       <c r="AD33" t="n">
-        <v>0.03900982591239303</v>
+        <v>0.03353416050936642</v>
       </c>
       <c r="AE33" t="n">
-        <v>0.03900982591239303</v>
+        <v>0.03353416050936642</v>
       </c>
     </row>
     <row r="34">
@@ -3664,7 +3664,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.002443638625745545</v>
+        <v>-0.002444554177782167</v>
       </c>
       <c r="D34" t="n">
         <v>0.01138237082329483</v>
@@ -3676,79 +3676,79 @@
         <v>0.004982926087317043</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.005139760429590416</v>
+        <v>-0.005139517453580697</v>
       </c>
       <c r="H34" t="n">
         <v>-0.0001791087431643497</v>
       </c>
       <c r="I34" t="n">
-        <v>0.006501060260042409</v>
+        <v>0.006530188389207534</v>
       </c>
       <c r="J34" t="n">
-        <v>0.009344848224783471</v>
+        <v>0.009444458890551715</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01041866768074671</v>
+        <v>0.9201883739915349</v>
       </c>
       <c r="L34" t="n">
-        <v>0.01041866768074671</v>
+        <v>0.9201883739915349</v>
       </c>
       <c r="M34" t="n">
-        <v>0.01041866768074671</v>
+        <v>0.9201883739915349</v>
       </c>
       <c r="N34" t="n">
-        <v>0.01041866768074671</v>
+        <v>0.9201883739915349</v>
       </c>
       <c r="O34" t="n">
-        <v>0.01041866768074671</v>
+        <v>0.9201883739915349</v>
       </c>
       <c r="P34" t="n">
-        <v>0.005684744675389786</v>
+        <v>0.0976338853133554</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.008811348640453943</v>
+        <v>0.5299280937411237</v>
       </c>
       <c r="R34" t="n">
-        <v>0.008811348640453943</v>
+        <v>0.5299280937411237</v>
       </c>
       <c r="S34" t="n">
-        <v>0.008811348640453943</v>
+        <v>0.5299280937411237</v>
       </c>
       <c r="T34" t="n">
-        <v>0.008811348640453943</v>
+        <v>0.5299280937411237</v>
       </c>
       <c r="U34" t="n">
-        <v>0.01096701413468056</v>
+        <v>0.01097320719092829</v>
       </c>
       <c r="V34" t="n">
         <v>-0.01936147488645899</v>
       </c>
       <c r="W34" t="n">
-        <v>0.02621600322464012</v>
+        <v>0.02621589685663588</v>
       </c>
       <c r="X34" t="n">
-        <v>0.02158349155133966</v>
+        <v>0.02158084377523375</v>
       </c>
       <c r="Y34" t="n">
         <v>0.03202135779285431</v>
       </c>
       <c r="Z34" t="n">
-        <v>0.02210870411634816</v>
+        <v>0.02207927521917101</v>
       </c>
       <c r="AA34" t="n">
-        <v>-0.01730340702813628</v>
+        <v>-0.2769149887085995</v>
       </c>
       <c r="AB34" t="n">
-        <v>-0.01730340702813628</v>
+        <v>-0.2769149887085995</v>
       </c>
       <c r="AC34" t="n">
-        <v>-0.01730340702813628</v>
+        <v>-0.2769149887085995</v>
       </c>
       <c r="AD34" t="n">
-        <v>-0.01730340702813628</v>
+        <v>-0.2769149887085995</v>
       </c>
       <c r="AE34" t="n">
-        <v>-0.01730340702813628</v>
+        <v>-0.2769149887085995</v>
       </c>
     </row>
     <row r="35">
@@ -3763,7 +3763,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.02273296218931848</v>
+        <v>0.02273426231737049</v>
       </c>
       <c r="D35" t="n">
         <v>0.02218259157530366</v>
@@ -3775,79 +3775,79 @@
         <v>-0.01147808061912322</v>
       </c>
       <c r="G35" t="n">
-        <v>0.009363640406545616</v>
+        <v>0.009363490550539621</v>
       </c>
       <c r="H35" t="n">
         <v>0.009095099403803975</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01784609543384381</v>
+        <v>0.01784798068191923</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.02032061219672153</v>
+        <v>-0.0200613293500821</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.01304908544996342</v>
+        <v>-0.003154868478194739</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.01304908544996342</v>
+        <v>-0.003154868478194739</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.01304908544996342</v>
+        <v>-0.003154868478194739</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.01304908544996342</v>
+        <v>-0.003154868478194739</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.01304908544996342</v>
+        <v>-0.003154868478194739</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.01095659947826398</v>
+        <v>-0.01044453968178159</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.01426838351473534</v>
+        <v>-0.01094251790970071</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.01426838351473534</v>
+        <v>-0.01094251790970071</v>
       </c>
       <c r="S35" t="n">
-        <v>-0.01426838351473534</v>
+        <v>-0.01094251790970071</v>
       </c>
       <c r="T35" t="n">
-        <v>-0.01426838351473534</v>
+        <v>-0.01094251790970071</v>
       </c>
       <c r="U35" t="n">
-        <v>-0.01683305174532207</v>
+        <v>-0.01684139107365564</v>
       </c>
       <c r="V35" t="n">
         <v>0.01693082122123285</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.004210715112428604</v>
+        <v>-0.004210911432436457</v>
       </c>
       <c r="X35" t="n">
-        <v>-0.02909041988361679</v>
+        <v>-0.02909373821974953</v>
       </c>
       <c r="Y35" t="n">
         <v>-0.005420779992831199</v>
       </c>
       <c r="Z35" t="n">
-        <v>-0.02808919437156777</v>
+        <v>-0.02806639533065581</v>
       </c>
       <c r="AA35" t="n">
-        <v>0.024913400004536</v>
+        <v>0.02310082124403285</v>
       </c>
       <c r="AB35" t="n">
-        <v>0.024913400004536</v>
+        <v>0.02310082124403285</v>
       </c>
       <c r="AC35" t="n">
-        <v>0.024913400004536</v>
+        <v>0.02310082124403285</v>
       </c>
       <c r="AD35" t="n">
-        <v>0.024913400004536</v>
+        <v>0.02310082124403285</v>
       </c>
       <c r="AE35" t="n">
-        <v>0.024913400004536</v>
+        <v>0.02310082124403285</v>
       </c>
     </row>
     <row r="36">
@@ -3862,7 +3862,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.04354365582174623</v>
+        <v>0.04352945934117837</v>
       </c>
       <c r="D36" t="n">
         <v>-0.002515635364625415</v>
@@ -3874,79 +3874,79 @@
         <v>-0.03067577633103105</v>
       </c>
       <c r="G36" t="n">
-        <v>0.03049929865997194</v>
+        <v>0.03049941894797675</v>
       </c>
       <c r="H36" t="n">
         <v>0.02943817711352708</v>
       </c>
       <c r="I36" t="n">
-        <v>0.00835192353407694</v>
+        <v>0.008361885166475406</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.01926560527328056</v>
+        <v>-0.0194495213245232</v>
       </c>
       <c r="K36" t="n">
-        <v>0.2476104161444166</v>
+        <v>0.07459743053589721</v>
       </c>
       <c r="L36" t="n">
-        <v>0.2476104161444166</v>
+        <v>0.07459743053589721</v>
       </c>
       <c r="M36" t="n">
-        <v>0.2476104161444166</v>
+        <v>0.07459743053589721</v>
       </c>
       <c r="N36" t="n">
-        <v>0.2476104161444166</v>
+        <v>0.07459743053589721</v>
       </c>
       <c r="O36" t="n">
-        <v>0.2476104161444166</v>
+        <v>0.07459743053589721</v>
       </c>
       <c r="P36" t="n">
-        <v>-0.01955149537405981</v>
+        <v>-0.02183987156159486</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.05071372772454911</v>
+        <v>0.02359831409593256</v>
       </c>
       <c r="R36" t="n">
-        <v>0.05071372772454911</v>
+        <v>0.02359831409593256</v>
       </c>
       <c r="S36" t="n">
-        <v>0.05071372772454911</v>
+        <v>0.02359831409593256</v>
       </c>
       <c r="T36" t="n">
-        <v>0.05071372772454911</v>
+        <v>0.02359831409593256</v>
       </c>
       <c r="U36" t="n">
-        <v>0.007239642721585707</v>
+        <v>0.00727767177910687</v>
       </c>
       <c r="V36" t="n">
         <v>-0.0008818497952739917</v>
       </c>
       <c r="W36" t="n">
-        <v>-0.02650916477236659</v>
+        <v>-0.02650900416436016</v>
       </c>
       <c r="X36" t="n">
-        <v>-0.006300162396006495</v>
+        <v>-0.006303913308156532</v>
       </c>
       <c r="Y36" t="n">
         <v>0.002575499815019992</v>
       </c>
       <c r="Z36" t="n">
-        <v>-0.01464210682568427</v>
+        <v>-0.01497865979914639</v>
       </c>
       <c r="AA36" t="n">
-        <v>0.1349936177517447</v>
+        <v>0.1232792794911712</v>
       </c>
       <c r="AB36" t="n">
-        <v>0.1349936177517447</v>
+        <v>0.1232792794911712</v>
       </c>
       <c r="AC36" t="n">
-        <v>0.1349936177517447</v>
+        <v>0.1232792794911712</v>
       </c>
       <c r="AD36" t="n">
-        <v>0.1349936177517447</v>
+        <v>0.1232792794911712</v>
       </c>
       <c r="AE36" t="n">
-        <v>0.1349936177517447</v>
+        <v>0.1232792794911712</v>
       </c>
     </row>
     <row r="37">
@@ -3961,7 +3961,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.0128545901141836</v>
+        <v>0.01284706332988253</v>
       </c>
       <c r="D37" t="n">
         <v>-0.01464582970583318</v>
@@ -3973,79 +3973,79 @@
         <v>-0.01999151897566076</v>
       </c>
       <c r="G37" t="n">
-        <v>0.02122357851294314</v>
+        <v>0.02122339649693586</v>
       </c>
       <c r="H37" t="n">
         <v>0.02265021402600856</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.001623945568957823</v>
+        <v>-0.001597213407888536</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.004710341617953026</v>
+        <v>-0.003734189915999518</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.001689639043585562</v>
+        <v>-0.01505527567421103</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.001689639043585562</v>
+        <v>-0.01505527567421103</v>
       </c>
       <c r="M37" t="n">
-        <v>-0.001689639043585562</v>
+        <v>-0.01505527567421103</v>
       </c>
       <c r="N37" t="n">
-        <v>-0.001689639043585562</v>
+        <v>-0.01505527567421103</v>
       </c>
       <c r="O37" t="n">
-        <v>-0.001689639043585562</v>
+        <v>-0.01505527567421103</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.01984733205789328</v>
+        <v>-0.02132136037285441</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.01386722321068893</v>
+        <v>-0.02145098370603934</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.01386722321068893</v>
+        <v>-0.02145098370603934</v>
       </c>
       <c r="S37" t="n">
-        <v>-0.01386722321068893</v>
+        <v>-0.02145098370603934</v>
       </c>
       <c r="T37" t="n">
-        <v>-0.01386722321068893</v>
+        <v>-0.02145098370603934</v>
       </c>
       <c r="U37" t="n">
-        <v>-0.02047925390717015</v>
+        <v>-0.02045462453018498</v>
       </c>
       <c r="V37" t="n">
         <v>-0.01445076163403046</v>
       </c>
       <c r="W37" t="n">
-        <v>0.009300339540013582</v>
+        <v>0.009301338132053524</v>
       </c>
       <c r="X37" t="n">
-        <v>-0.003962256542490261</v>
+        <v>-0.003955690910227636</v>
       </c>
       <c r="Y37" t="n">
         <v>0.01697723290308931</v>
       </c>
       <c r="Z37" t="n">
-        <v>-0.01338772863150914</v>
+        <v>-0.01352238054089522</v>
       </c>
       <c r="AA37" t="n">
-        <v>0.009854064970162599</v>
+        <v>0.01346501938660078</v>
       </c>
       <c r="AB37" t="n">
-        <v>0.009854064970162599</v>
+        <v>0.01346501938660078</v>
       </c>
       <c r="AC37" t="n">
-        <v>0.009854064970162599</v>
+        <v>0.01346501938660078</v>
       </c>
       <c r="AD37" t="n">
-        <v>0.009854064970162599</v>
+        <v>0.01346501938660078</v>
       </c>
       <c r="AE37" t="n">
-        <v>0.009854064970162599</v>
+        <v>0.01346501938660078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continue running and setup KDE plots
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_1.xlsx
@@ -734,10 +734,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.08820291050411641</v>
+        <v>-0.08819368922374757</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.002222304185919323</v>
+        <v>-0.0007841772737814185</v>
       </c>
       <c r="E4" t="n">
         <v>-0.1177646069825843</v>
@@ -752,10 +752,10 @@
         <v>0.1765836888553475</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0517564951262598</v>
+        <v>0.05172981173319247</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09460332107991955</v>
+        <v>0.09460357039192963</v>
       </c>
       <c r="K4" t="n">
         <v>0.3218543532581741</v>
@@ -788,37 +788,37 @@
         <v>0.2157335591893423</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.09716265364650613</v>
+        <v>-0.09716239742249587</v>
       </c>
       <c r="V4" t="n">
         <v>-0.7014339902653596</v>
       </c>
       <c r="W4" t="n">
-        <v>0.01957704481508179</v>
+        <v>0.01957573345502934</v>
       </c>
       <c r="X4" t="n">
-        <v>0.277196949935878</v>
+        <v>0.2769967113998684</v>
       </c>
       <c r="Y4" t="n">
         <v>0.9980585371063413</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.1876748669949946</v>
+        <v>0.1879505613420224</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.1378479537059181</v>
+        <v>0.1378275919131037</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.1378479537059181</v>
+        <v>0.1378275919131037</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.1378479537059181</v>
+        <v>0.1378275919131037</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.1378479537059181</v>
+        <v>0.1378275919131037</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.1378479537059181</v>
+        <v>0.1378275919131037</v>
       </c>
     </row>
     <row r="5">
@@ -829,10 +829,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1108973797638952</v>
+        <v>0.1108998349639934</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0246776916950735</v>
+        <v>0.02235322168801487</v>
       </c>
       <c r="E5" t="n">
         <v>0.1433098626923945</v>
@@ -847,10 +847,10 @@
         <v>0.008470465394818614</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.04609968318798732</v>
+        <v>-0.04609942590797703</v>
       </c>
       <c r="J5" t="n">
-        <v>0.03058196907355431</v>
+        <v>0.03058229566556748</v>
       </c>
       <c r="K5" t="n">
         <v>-0.1744807564512302</v>
@@ -883,37 +883,37 @@
         <v>-0.06032707479708298</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1132901837956073</v>
+        <v>0.1132905333316213</v>
       </c>
       <c r="V5" t="n">
         <v>0.6536887663075507</v>
       </c>
       <c r="W5" t="n">
-        <v>0.002549239589969583</v>
+        <v>0.002550984582039383</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.2094055566002223</v>
+        <v>-0.2093316953492678</v>
       </c>
       <c r="Y5" t="n">
         <v>-0.01176007064640282</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.1325776770471071</v>
+        <v>-0.1324872278594891</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.1189811379432455</v>
+        <v>-0.1190020324400813</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.1189811379432455</v>
+        <v>-0.1190020324400813</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.1189811379432455</v>
+        <v>-0.1190020324400813</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.1189811379432455</v>
+        <v>-0.1190020324400813</v>
       </c>
       <c r="AE5" t="n">
-        <v>-0.1189811379432455</v>
+        <v>-0.1190020324400813</v>
       </c>
     </row>
     <row r="6">
@@ -924,10 +924,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2847333148453326</v>
+        <v>0.28473625177345</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.009671582907876218</v>
+        <v>-0.0104059294804427</v>
       </c>
       <c r="E6" t="n">
         <v>-0.002243198393727935</v>
@@ -942,10 +942,10 @@
         <v>-0.006998576439943056</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.8951564883822594</v>
+        <v>-0.8951572899822914</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.003808967049638495</v>
+        <v>-0.003808890633635412</v>
       </c>
       <c r="K6" t="n">
         <v>0.03190318169212726</v>
@@ -978,37 +978,37 @@
         <v>0.04292297403691896</v>
       </c>
       <c r="U6" t="n">
-        <v>0.04984166215366648</v>
+        <v>0.04983527882541115</v>
       </c>
       <c r="V6" t="n">
         <v>0.02071473481258939</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.02798428825537153</v>
+        <v>-0.02798221609528864</v>
       </c>
       <c r="X6" t="n">
-        <v>0.004335077165403086</v>
+        <v>0.004546676917867076</v>
       </c>
       <c r="Y6" t="n">
         <v>-0.0009891643595665743</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.3582525850821034</v>
+        <v>-0.3580974490758979</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.02062284735291389</v>
+        <v>-0.02062697938507917</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.02062284735291389</v>
+        <v>-0.02062697938507917</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.02062284735291389</v>
+        <v>-0.02062697938507917</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.02062284735291389</v>
+        <v>-0.02062697938507917</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.02062284735291389</v>
+        <v>-0.02062697938507917</v>
       </c>
     </row>
     <row r="7">
@@ -1019,10 +1019,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.01634973876598955</v>
+        <v>0.01634850871794034</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01070557607023833</v>
+        <v>0.01237592717451917</v>
       </c>
       <c r="E7" t="n">
         <v>0.01175450811818032</v>
@@ -1037,10 +1037,10 @@
         <v>0.0088485200339408</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.001790539463621578</v>
+        <v>-0.001785953063438122</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.00605698459631453</v>
+        <v>-0.006056913076311645</v>
       </c>
       <c r="K7" t="n">
         <v>-0.01967494158699766</v>
@@ -1073,37 +1073,37 @@
         <v>-0.0184031150081246</v>
       </c>
       <c r="U7" t="n">
-        <v>0.01743797618551905</v>
+        <v>0.01744079829763193</v>
       </c>
       <c r="V7" t="n">
         <v>0.007844667961786718</v>
       </c>
       <c r="W7" t="n">
-        <v>0.01725052129802085</v>
+        <v>0.01725245301009812</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.0184023151360926</v>
+        <v>-0.01837238943889558</v>
       </c>
       <c r="Y7" t="n">
         <v>-0.01073606452544258</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.01233246039729841</v>
+        <v>-0.01238691870347675</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.01271250473250019</v>
+        <v>0.01271976041279041</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.01271250473250019</v>
+        <v>0.01271976041279041</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.01271250473250019</v>
+        <v>0.01271976041279041</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.01271250473250019</v>
+        <v>0.01271976041279041</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.01271250473250019</v>
+        <v>0.01271976041279041</v>
       </c>
     </row>
     <row r="8">
@@ -1114,10 +1114,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.01291597107663884</v>
+        <v>0.01291640643665625</v>
       </c>
       <c r="D8" t="n">
-        <v>0.003029323358537903</v>
+        <v>0.003168876215948515</v>
       </c>
       <c r="E8" t="n">
         <v>-0.001420882808835312</v>
@@ -1132,10 +1132,10 @@
         <v>-0.001561537790461512</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.01070253546810142</v>
+        <v>-0.01070332401213296</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.001695292004381298</v>
+        <v>-0.001695279428380791</v>
       </c>
       <c r="K8" t="n">
         <v>0.01009325934773037</v>
@@ -1168,37 +1168,37 @@
         <v>0.01192678598107144</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.003447760553910422</v>
+        <v>-0.003473240970929638</v>
       </c>
       <c r="V8" t="n">
         <v>-0.004322193676887747</v>
       </c>
       <c r="W8" t="n">
-        <v>0.009309082260363288</v>
+        <v>0.00930859381234375</v>
       </c>
       <c r="X8" t="n">
-        <v>0.001610521984420879</v>
+        <v>0.001255574834222993</v>
       </c>
       <c r="Y8" t="n">
         <v>0.003052186202087448</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.005145499693819987</v>
+        <v>0.005127576109103044</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.004678424347136973</v>
+        <v>-0.00463113301724532</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.004678424347136973</v>
+        <v>-0.00463113301724532</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.004678424347136973</v>
+        <v>-0.00463113301724532</v>
       </c>
       <c r="AD8" t="n">
-        <v>-0.004678424347136973</v>
+        <v>-0.00463113301724532</v>
       </c>
       <c r="AE8" t="n">
-        <v>-0.004678424347136973</v>
+        <v>-0.00463113301724532</v>
       </c>
     </row>
     <row r="9">
@@ -1213,10 +1213,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4711520425260817</v>
+        <v>0.4711518555180741</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01333991288318761</v>
+        <v>0.01440663000468191</v>
       </c>
       <c r="E9" t="n">
         <v>0.003303209604128384</v>
@@ -1231,10 +1231,10 @@
         <v>0.000364514126580565</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.01151166410846656</v>
+        <v>-0.01151155054046202</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.01266347292679384</v>
+        <v>-0.01266383091080828</v>
       </c>
       <c r="K9" t="n">
         <v>-0.01695037824601513</v>
@@ -1267,37 +1267,37 @@
         <v>-0.01515954771038191</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.6016127738565108</v>
+        <v>-0.6016135453125417</v>
       </c>
       <c r="V9" t="n">
         <v>0.002256314106252564</v>
       </c>
       <c r="W9" t="n">
-        <v>0.009571917310876692</v>
+        <v>0.009573121438924857</v>
       </c>
       <c r="X9" t="n">
-        <v>-0.009597158111886323</v>
+        <v>-0.01016562645462506</v>
       </c>
       <c r="Y9" t="n">
         <v>-0.002613878696555147</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.001450084666003386</v>
+        <v>-0.001565303486612139</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.007346808101872324</v>
+        <v>0.007418466728738669</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.007346808101872324</v>
+        <v>0.007418466728738669</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.007346808101872324</v>
+        <v>0.007418466728738669</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.007346808101872324</v>
+        <v>0.007418466728738669</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.007346808101872324</v>
+        <v>0.007418466728738669</v>
       </c>
     </row>
     <row r="10">
@@ -1312,10 +1312,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5412393346095733</v>
+        <v>0.5412418754416749</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.02533504719236338</v>
+        <v>-0.02502177167463026</v>
       </c>
       <c r="E10" t="n">
         <v>0.02868284956331398</v>
@@ -1330,10 +1330,10 @@
         <v>0.03064438672977546</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.004728405405136215</v>
+        <v>-0.004729843005193719</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01316338473895829</v>
+        <v>0.01316349974696292</v>
       </c>
       <c r="K10" t="n">
         <v>-0.02488873203554928</v>
@@ -1366,37 +1366,37 @@
         <v>-0.02843166670526666</v>
       </c>
       <c r="U10" t="n">
-        <v>0.6983664156466565</v>
+        <v>0.6983741012149639</v>
       </c>
       <c r="V10" t="n">
         <v>0.002660347114413884</v>
       </c>
       <c r="W10" t="n">
-        <v>0.005824842760993709</v>
+        <v>0.005826071849042874</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.009699288003971518</v>
+        <v>-0.009126661133066443</v>
       </c>
       <c r="Y10" t="n">
         <v>0.004826509345060373</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.02109401949976078</v>
+        <v>-0.02090100986004039</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.01459333959173358</v>
+        <v>0.01451968205278728</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.01459333959173358</v>
+        <v>0.01451968205278728</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.01459333959173358</v>
+        <v>0.01451968205278728</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.01459333959173358</v>
+        <v>0.01451968205278728</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.01459333959173358</v>
+        <v>0.01451968205278728</v>
       </c>
     </row>
     <row r="11">
@@ -1411,10 +1411,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.00231698975667959</v>
+        <v>-0.002314855484594219</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.00858675417118916</v>
+        <v>-0.01004341157558213</v>
       </c>
       <c r="E11" t="n">
         <v>0.002898114931924597</v>
@@ -1429,10 +1429,10 @@
         <v>-0.001071932202877288</v>
       </c>
       <c r="I11" t="n">
-        <v>0.003691442643657705</v>
+        <v>0.00368112926724517</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.01156025600229448</v>
+        <v>-0.01156008934628776</v>
       </c>
       <c r="K11" t="n">
         <v>-0.001577854527114181</v>
@@ -1465,37 +1465,37 @@
         <v>-0.0006282139451285577</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.0107901125276045</v>
+        <v>-0.01079165601566624</v>
       </c>
       <c r="V11" t="n">
         <v>-0.002020335824813433</v>
       </c>
       <c r="W11" t="n">
-        <v>0.01837746659109866</v>
+        <v>0.01837681686307267</v>
       </c>
       <c r="X11" t="n">
-        <v>0.01064774730590989</v>
+        <v>0.01068700794748032</v>
       </c>
       <c r="Y11" t="n">
         <v>-0.01424356280974251</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.005051407498056299</v>
+        <v>-0.005130832813233312</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.008439303217572127</v>
+        <v>-0.00843379425735177</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.008439303217572127</v>
+        <v>-0.00843379425735177</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.008439303217572127</v>
+        <v>-0.00843379425735177</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.008439303217572127</v>
+        <v>-0.00843379425735177</v>
       </c>
       <c r="AE11" t="n">
-        <v>-0.008439303217572127</v>
+        <v>-0.00843379425735177</v>
       </c>
     </row>
     <row r="12">
@@ -1510,10 +1510,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.08083895891355834</v>
+        <v>0.08084060963362437</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.01914018769880638</v>
+        <v>-0.01596015271055784</v>
       </c>
       <c r="E12" t="n">
         <v>0.008717855484714218</v>
@@ -1528,10 +1528,10 @@
         <v>0.01309334375573375</v>
       </c>
       <c r="I12" t="n">
-        <v>0.01171549544461981</v>
+        <v>0.01170848206833928</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.02390575291626245</v>
+        <v>-0.02390579419626411</v>
       </c>
       <c r="K12" t="n">
         <v>0.004082965987318639</v>
@@ -1564,37 +1564,37 @@
         <v>0.001518869916754797</v>
       </c>
       <c r="U12" t="n">
-        <v>0.07105063791402551</v>
+        <v>0.07107876677915066</v>
       </c>
       <c r="V12" t="n">
         <v>-0.0149328974613159</v>
       </c>
       <c r="W12" t="n">
-        <v>0.0283026176441047</v>
+        <v>0.02830058071602323</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.003986461599458463</v>
+        <v>-0.003677877843115114</v>
       </c>
       <c r="Y12" t="n">
         <v>0.01068090839523633</v>
       </c>
       <c r="Z12" t="n">
-        <v>-0.02508790813951632</v>
+        <v>-0.02506821825072873</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.01652115186084607</v>
+        <v>0.01646708110668324</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.01652115186084607</v>
+        <v>0.01646708110668324</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.01652115186084607</v>
+        <v>0.01646708110668324</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.01652115186084607</v>
+        <v>0.01646708110668324</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.01652115186084607</v>
+        <v>0.01646708110668324</v>
       </c>
     </row>
     <row r="13">
@@ -1605,10 +1605,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.3360778912351156</v>
+        <v>-0.3360782448991297</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01495608251339567</v>
+        <v>0.01421524514084199</v>
       </c>
       <c r="E13" t="n">
         <v>0.0126909301716372</v>
@@ -1623,10 +1623,10 @@
         <v>0.01952371537294861</v>
       </c>
       <c r="I13" t="n">
-        <v>0.009617064384682574</v>
+        <v>0.009623351904934074</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0128564434945775</v>
+        <v>0.01285657655058287</v>
       </c>
       <c r="K13" t="n">
         <v>0.006689155755566229</v>
@@ -1659,37 +1659,37 @@
         <v>0.001644503201780128</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.07304021572160863</v>
+        <v>-0.07304650957786038</v>
       </c>
       <c r="V13" t="n">
         <v>-0.01589750396390015</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.009640837825633511</v>
+        <v>-0.009640773985630957</v>
       </c>
       <c r="X13" t="n">
-        <v>7.050153882006153e-05</v>
+        <v>4.36344977453799e-05</v>
       </c>
       <c r="Y13" t="n">
         <v>0.0127554426542177</v>
       </c>
       <c r="Z13" t="n">
-        <v>-0.008871034722841389</v>
+        <v>-0.008932201221288046</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.009882931307317251</v>
+        <v>0.009903543564141741</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.009882931307317251</v>
+        <v>0.009903543564141741</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.009882931307317251</v>
+        <v>0.009903543564141741</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.009882931307317251</v>
+        <v>0.009903543564141741</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.009882931307317251</v>
+        <v>0.009903543564141741</v>
       </c>
     </row>
     <row r="14">
@@ -1704,10 +1704,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.008888892643555704</v>
+        <v>0.008888047939521916</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.008997356194296082</v>
+        <v>-0.00607027732474943</v>
       </c>
       <c r="E14" t="n">
         <v>0.0045449974937999</v>
@@ -1722,10 +1722,10 @@
         <v>0.0074490650019626</v>
       </c>
       <c r="I14" t="n">
-        <v>0.001016052904642116</v>
+        <v>0.001022284072891363</v>
       </c>
       <c r="J14" t="n">
-        <v>0.01415804466707889</v>
+        <v>0.01415779189906869</v>
       </c>
       <c r="K14" t="n">
         <v>-0.01020048540001941</v>
@@ -1758,37 +1758,37 @@
         <v>-0.01127541136301645</v>
       </c>
       <c r="U14" t="n">
-        <v>0.02041355361654214</v>
+        <v>0.02040373473614939</v>
       </c>
       <c r="V14" t="n">
         <v>-0.006572320294892811</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.0001623593344943734</v>
+        <v>-0.0001610116864404674</v>
       </c>
       <c r="X14" t="n">
-        <v>0.007893215643728625</v>
+        <v>0.00813498378139935</v>
       </c>
       <c r="Y14" t="n">
         <v>-0.003784722487388899</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.004016935552677421</v>
+        <v>-0.003851766874070675</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.0007360727334429093</v>
+        <v>0.0007340590373623614</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.0007360727334429093</v>
+        <v>0.0007340590373623614</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.0007360727334429093</v>
+        <v>0.0007340590373623614</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.0007360727334429093</v>
+        <v>0.0007340590373623614</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.0007360727334429093</v>
+        <v>0.0007340590373623614</v>
       </c>
     </row>
     <row r="15">
@@ -1803,10 +1803,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.03621448877657955</v>
+        <v>-0.0362139101845564</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.02150100949324983</v>
+        <v>-0.01912815111237276</v>
       </c>
       <c r="E15" t="n">
         <v>0.005581299775251989</v>
@@ -1821,10 +1821,10 @@
         <v>0.005684687939387516</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0159771101430844</v>
+        <v>0.01596955407878216</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.01890361655449628</v>
+        <v>-0.01890337559448656</v>
       </c>
       <c r="K15" t="n">
         <v>0.003145142909805716</v>
@@ -1857,37 +1857,37 @@
         <v>0.003110477212419088</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.0531154400766176</v>
+        <v>-0.05311335745253429</v>
       </c>
       <c r="V15" t="n">
         <v>0.001012833160513326</v>
       </c>
       <c r="W15" t="n">
-        <v>0.00264778848991154</v>
+        <v>0.002647746921909876</v>
       </c>
       <c r="X15" t="n">
-        <v>-0.009327843829113752</v>
+        <v>-0.009156907854276312</v>
       </c>
       <c r="Y15" t="n">
         <v>0.001504486524179461</v>
       </c>
       <c r="Z15" t="n">
-        <v>-0.005529244733169789</v>
+        <v>-0.005307383828295352</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.002140020277600811</v>
+        <v>0.002119870548794821</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.002140020277600811</v>
+        <v>0.002119870548794821</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.002140020277600811</v>
+        <v>0.002119870548794821</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.002140020277600811</v>
+        <v>0.002119870548794821</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.002140020277600811</v>
+        <v>0.002119870548794821</v>
       </c>
     </row>
     <row r="16">
@@ -1902,10 +1902,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.01377365930294637</v>
+        <v>0.0137726899909076</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02882205460098497</v>
+        <v>-0.02775181444280391</v>
       </c>
       <c r="E16" t="n">
         <v>0.003440934185637367</v>
@@ -1920,10 +1920,10 @@
         <v>0.004056001122240045</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.02390144822005793</v>
+        <v>-0.02389937701997508</v>
       </c>
       <c r="J16" t="n">
-        <v>0.001035991817787766</v>
+        <v>0.001036187369795654</v>
       </c>
       <c r="K16" t="n">
         <v>0.02383328879333155</v>
@@ -1956,37 +1956,37 @@
         <v>0.02306301596252064</v>
       </c>
       <c r="U16" t="n">
-        <v>0.008962567462502697</v>
+        <v>0.008948753061950122</v>
       </c>
       <c r="V16" t="n">
         <v>0.0002018855120754205</v>
       </c>
       <c r="W16" t="n">
-        <v>0.01410769093230763</v>
+        <v>0.01410884773235391</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.009740809445632376</v>
+        <v>-0.009977974671118986</v>
       </c>
       <c r="Y16" t="n">
         <v>0.00116841326273653</v>
       </c>
       <c r="Z16" t="n">
-        <v>-0.02589701882788075</v>
+        <v>-0.02590620055624802</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.005988286223531448</v>
+        <v>0.006021865008874598</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.005988286223531448</v>
+        <v>0.006021865008874598</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.005988286223531448</v>
+        <v>0.006021865008874598</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.005988286223531448</v>
+        <v>0.006021865008874598</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.005988286223531448</v>
+        <v>0.006021865008874598</v>
       </c>
     </row>
     <row r="17">
@@ -2001,10 +2001,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.02116980641479226</v>
+        <v>-0.02116983790279351</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01958263626867382</v>
+        <v>0.01923196868291192</v>
       </c>
       <c r="E17" t="n">
         <v>0.003722611156904446</v>
@@ -2019,10 +2019,10 @@
         <v>0.008068310050732401</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.01130640237225609</v>
+        <v>-0.01131324112452964</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.01183988730957369</v>
+        <v>-0.01184005454158044</v>
       </c>
       <c r="K17" t="n">
         <v>-0.001667809410712376</v>
@@ -2055,37 +2055,37 @@
         <v>-0.003665225234609009</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.01651324050052962</v>
+        <v>-0.01649151051566042</v>
       </c>
       <c r="V17" t="n">
         <v>-0.009309831060393242</v>
       </c>
       <c r="W17" t="n">
-        <v>0.01908738479549539</v>
+        <v>0.01908567618742705</v>
       </c>
       <c r="X17" t="n">
-        <v>0.001445365401814616</v>
+        <v>0.001653186114127444</v>
       </c>
       <c r="Y17" t="n">
         <v>0.01156044468641779</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.0004429572657182906</v>
+        <v>0.0003579918863196754</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.007348763333950533</v>
+        <v>0.007316560132662404</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.007348763333950533</v>
+        <v>0.007316560132662404</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.007348763333950533</v>
+        <v>0.007316560132662404</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.007348763333950533</v>
+        <v>0.007316560132662404</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.007348763333950533</v>
+        <v>0.007316560132662404</v>
       </c>
     </row>
     <row r="18">
@@ -2096,10 +2096,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.01298631661545266</v>
+        <v>-0.01298604915944196</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02385733805392157</v>
+        <v>0.02198905814405584</v>
       </c>
       <c r="E18" t="n">
         <v>0.002900400980016038</v>
@@ -2114,10 +2114,10 @@
         <v>0.017880824971233</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.001509100668364026</v>
+        <v>-0.001513981308559252</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.0182047527023069</v>
+        <v>-0.01820462070230158</v>
       </c>
       <c r="K18" t="n">
         <v>0.01201746201669848</v>
@@ -2150,37 +2150,37 @@
         <v>0.005411056248442249</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.01364175116967004</v>
+        <v>-0.01361601702464068</v>
       </c>
       <c r="V18" t="n">
         <v>-0.04053771522150861</v>
       </c>
       <c r="W18" t="n">
-        <v>-0.01218653549546142</v>
+        <v>-0.01218734218349369</v>
       </c>
       <c r="X18" t="n">
-        <v>0.006122459092898364</v>
+        <v>0.00656860077474403</v>
       </c>
       <c r="Y18" t="n">
         <v>0.03970474469218978</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.01554156330966253</v>
+        <v>0.01568793941151757</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.01985579839423193</v>
+        <v>0.01978761650350466</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.01985579839423193</v>
+        <v>0.01978761650350466</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.01985579839423193</v>
+        <v>0.01978761650350466</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.01985579839423193</v>
+        <v>0.01978761650350466</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.01985579839423193</v>
+        <v>0.01978761650350466</v>
       </c>
     </row>
     <row r="19">
@@ -2195,10 +2195,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.01222268295290732</v>
+        <v>0.01222106036084241</v>
       </c>
       <c r="D19" t="n">
-        <v>0.02731273216695289</v>
+        <v>0.02577546403210559</v>
       </c>
       <c r="E19" t="n">
         <v>0.01844926576197063</v>
@@ -2213,10 +2213,10 @@
         <v>0.01502727324109093</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0152373050254922</v>
+        <v>0.01524797177791887</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0003724788150243055</v>
+        <v>0.0003725193270259395</v>
       </c>
       <c r="K19" t="n">
         <v>-0.02914314039772561</v>
@@ -2249,37 +2249,37 @@
         <v>-0.0277766427430657</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.005419947864797913</v>
+        <v>-0.005398901687956067</v>
       </c>
       <c r="V19" t="n">
         <v>0.01622704192908168</v>
       </c>
       <c r="W19" t="n">
-        <v>0.006967646678705866</v>
+        <v>0.006969067862762713</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.005479502331180093</v>
+        <v>-0.005058547786341911</v>
       </c>
       <c r="Y19" t="n">
         <v>-0.008200182472007298</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.001658465538338622</v>
+        <v>0.00184601700184068</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.01364291142571646</v>
+        <v>0.01358121270324851</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.01364291142571646</v>
+        <v>0.01358121270324851</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.01364291142571646</v>
+        <v>0.01358121270324851</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.01364291142571646</v>
+        <v>0.01358121270324851</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.01364291142571646</v>
+        <v>0.01358121270324851</v>
       </c>
     </row>
     <row r="20">
@@ -2294,10 +2294,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.01138759696750388</v>
+        <v>-0.01138749328749973</v>
       </c>
       <c r="D20" t="n">
-        <v>0.003683503408177826</v>
+        <v>0.003174243082027346</v>
       </c>
       <c r="E20" t="n">
         <v>0.01143747674549907</v>
@@ -2312,10 +2312,10 @@
         <v>0.01584765816990633</v>
       </c>
       <c r="I20" t="n">
-        <v>0.006909315924372636</v>
+        <v>0.006913265172530606</v>
       </c>
       <c r="J20" t="n">
-        <v>0.01713665622722417</v>
+        <v>0.0171368107872304</v>
       </c>
       <c r="K20" t="n">
         <v>-0.01113558025342321</v>
@@ -2348,37 +2348,37 @@
         <v>-0.01402435217697409</v>
       </c>
       <c r="U20" t="n">
-        <v>0.00369821649992866</v>
+        <v>0.003715886164635446</v>
       </c>
       <c r="V20" t="n">
         <v>-0.008786878719475148</v>
       </c>
       <c r="W20" t="n">
-        <v>0.006263224090528962</v>
+        <v>0.00626379778655191</v>
       </c>
       <c r="X20" t="n">
-        <v>0.00537487451899498</v>
+        <v>0.005669314018772561</v>
       </c>
       <c r="Y20" t="n">
         <v>0.014574650118986</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.001347057173882287</v>
+        <v>0.001526444221057769</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.008361808654472346</v>
+        <v>0.008313374156534966</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.008361808654472346</v>
+        <v>0.008313374156534966</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.008361808654472346</v>
+        <v>0.008313374156534966</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.008361808654472346</v>
+        <v>0.008313374156534966</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.008361808654472346</v>
+        <v>0.008313374156534966</v>
       </c>
     </row>
     <row r="21">
@@ -2389,10 +2389,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.01012437218097489</v>
+        <v>-0.01012290894891636</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.006715809384285626</v>
+        <v>-0.007096920326507382</v>
       </c>
       <c r="E21" t="n">
         <v>0.01635339934213597</v>
@@ -2407,10 +2407,10 @@
         <v>0.01596776022271041</v>
       </c>
       <c r="I21" t="n">
-        <v>0.02666384593055383</v>
+        <v>0.02666007101840283</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.01591708576203157</v>
+        <v>-0.01591714221003385</v>
       </c>
       <c r="K21" t="n">
         <v>-0.004382890351315613</v>
@@ -2443,37 +2443,37 @@
         <v>-0.00452729451709178</v>
       </c>
       <c r="U21" t="n">
-        <v>-0.005391032087641283</v>
+        <v>-0.005374527862981114</v>
       </c>
       <c r="V21" t="n">
         <v>-0.001069568490782739</v>
       </c>
       <c r="W21" t="n">
-        <v>0.00395449177417967</v>
+        <v>0.003953571518142861</v>
       </c>
       <c r="X21" t="n">
-        <v>-0.01993094450923778</v>
+        <v>-0.01991072105242884</v>
       </c>
       <c r="Y21" t="n">
         <v>0.0103644024305761</v>
       </c>
       <c r="Z21" t="n">
-        <v>-0.01176034453441378</v>
+        <v>-0.01180958658438346</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.02317428361497134</v>
+        <v>0.02315653935826157</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.02317428361497134</v>
+        <v>0.02315653935826157</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.02317428361497134</v>
+        <v>0.02315653935826157</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.02317428361497134</v>
+        <v>0.02315653935826157</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.02317428361497134</v>
+        <v>0.02315653935826157</v>
       </c>
     </row>
     <row r="22">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.03008809973152398</v>
+        <v>-0.03008974872358994</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.006875211222745797</v>
+        <v>-0.006688834685262137</v>
       </c>
       <c r="E22" t="n">
         <v>-0.003770082774803311</v>
@@ -2502,10 +2502,10 @@
         <v>-0.002924413364976535</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.0001083964843358594</v>
+        <v>-0.0001058232042329281</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.00762874230771295</v>
+        <v>-0.007628710627711671</v>
       </c>
       <c r="K22" t="n">
         <v>-0.03361128076845122</v>
@@ -2538,37 +2538,37 @@
         <v>-0.03466837060273482</v>
       </c>
       <c r="U22" t="n">
-        <v>0.009185844175433765</v>
+        <v>0.00917290529491621</v>
       </c>
       <c r="V22" t="n">
         <v>0.001886523819460952</v>
       </c>
       <c r="W22" t="n">
-        <v>0.001630059329202373</v>
+        <v>0.001628181857127274</v>
       </c>
       <c r="X22" t="n">
-        <v>-0.01656090411843616</v>
+        <v>-0.01653790798951632</v>
       </c>
       <c r="Y22" t="n">
         <v>-0.002329811037192441</v>
       </c>
       <c r="Z22" t="n">
-        <v>-0.01386140993045639</v>
+        <v>-0.01393697335747893</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.02012738787709551</v>
+        <v>0.02014093568563742</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.02012738787709551</v>
+        <v>0.02014093568563742</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.02012738787709551</v>
+        <v>0.02014093568563742</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.02012738787709551</v>
+        <v>0.02014093568563742</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.02012738787709551</v>
+        <v>0.02014093568563742</v>
       </c>
     </row>
     <row r="23">
@@ -2579,10 +2579,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.01217157283886291</v>
+        <v>-0.01217308167092327</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000277861652598964</v>
+        <v>-0.0005731265125564069</v>
       </c>
       <c r="E23" t="n">
         <v>-0.00802029228881169</v>
@@ -2597,10 +2597,10 @@
         <v>-0.01048538873941555</v>
       </c>
       <c r="I23" t="n">
-        <v>0.003310613700424547</v>
+        <v>0.003318742692749707</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.004648344235495613</v>
+        <v>-0.00464825937149219</v>
       </c>
       <c r="K23" t="n">
         <v>0.005423250168930006</v>
@@ -2633,37 +2633,37 @@
         <v>0.005944524429780976</v>
       </c>
       <c r="U23" t="n">
-        <v>-0.007068435354737414</v>
+        <v>-0.007058065434322617</v>
       </c>
       <c r="V23" t="n">
         <v>0.008103711492148457</v>
       </c>
       <c r="W23" t="n">
-        <v>-0.002220205336808213</v>
+        <v>-0.00221887650475506</v>
       </c>
       <c r="X23" t="n">
-        <v>0.001332046325281853</v>
+        <v>0.001100442476017699</v>
       </c>
       <c r="Y23" t="n">
         <v>-0.007362674502506979</v>
       </c>
       <c r="Z23" t="n">
-        <v>-0.01773515149340606</v>
+        <v>-0.01782086624883465</v>
       </c>
       <c r="AA23" t="n">
-        <v>-0.004127681829107273</v>
+        <v>-0.004130088645203546</v>
       </c>
       <c r="AB23" t="n">
-        <v>-0.004127681829107273</v>
+        <v>-0.004130088645203546</v>
       </c>
       <c r="AC23" t="n">
-        <v>-0.004127681829107273</v>
+        <v>-0.004130088645203546</v>
       </c>
       <c r="AD23" t="n">
-        <v>-0.004127681829107273</v>
+        <v>-0.004130088645203546</v>
       </c>
       <c r="AE23" t="n">
-        <v>-0.004127681829107273</v>
+        <v>-0.004130088645203546</v>
       </c>
     </row>
     <row r="24">
@@ -2678,10 +2678,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.01976033992641359</v>
+        <v>-0.0197578424863137</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.004114019652691496</v>
+        <v>-0.002679691259643273</v>
       </c>
       <c r="E24" t="n">
         <v>0.00545126777005071</v>
@@ -2696,10 +2696,10 @@
         <v>0.007708004468320179</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.00312340226893609</v>
+        <v>-0.003124027228961089</v>
       </c>
       <c r="J24" t="n">
-        <v>0.004023543954293668</v>
+        <v>0.00402374257830168</v>
       </c>
       <c r="K24" t="n">
         <v>0.01220726688829067</v>
@@ -2732,37 +2732,37 @@
         <v>0.01011881954075278</v>
       </c>
       <c r="U24" t="n">
-        <v>0.01421068069642723</v>
+        <v>0.01421699336867973</v>
       </c>
       <c r="V24" t="n">
         <v>-0.01253947672557907</v>
       </c>
       <c r="W24" t="n">
-        <v>0.006858790450351616</v>
+        <v>0.006857633650305345</v>
       </c>
       <c r="X24" t="n">
-        <v>-0.00840913876836555</v>
+        <v>-0.008558945718357826</v>
       </c>
       <c r="Y24" t="n">
         <v>0.01078384900735396</v>
       </c>
       <c r="Z24" t="n">
-        <v>-0.01041320614452824</v>
+        <v>-0.01029931980397279</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.01165769777830791</v>
+        <v>0.01163954292958172</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.01165769777830791</v>
+        <v>0.01163954292958172</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.01165769777830791</v>
+        <v>0.01163954292958172</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.01165769777830791</v>
+        <v>0.01163954292958172</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.01165769777830791</v>
+        <v>0.01163954292958172</v>
       </c>
     </row>
     <row r="25">
@@ -2773,10 +2773,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.005754734054189361</v>
+        <v>-0.005752825574113022</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.01301323729658655</v>
+        <v>-0.01027155835410732</v>
       </c>
       <c r="E25" t="n">
         <v>0.01686670886666835</v>
@@ -2791,10 +2791,10 @@
         <v>0.02447870469114818</v>
       </c>
       <c r="I25" t="n">
-        <v>0.02399151801566072</v>
+        <v>0.02398887148755486</v>
       </c>
       <c r="J25" t="n">
-        <v>0.009410846443595902</v>
+        <v>0.009410766763592687</v>
       </c>
       <c r="K25" t="n">
         <v>-0.006226659609066384</v>
@@ -2827,37 +2827,37 @@
         <v>-0.01207992528319701</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.01103578095343124</v>
+        <v>-0.01104600456984018</v>
       </c>
       <c r="V25" t="n">
         <v>-0.01986577385063095</v>
       </c>
       <c r="W25" t="n">
-        <v>0.0178840876273635</v>
+        <v>0.01788427713137108</v>
       </c>
       <c r="X25" t="n">
-        <v>-0.01489077313963092</v>
+        <v>-0.01539021402360856</v>
       </c>
       <c r="Y25" t="n">
         <v>0.01503481279339251</v>
       </c>
       <c r="Z25" t="n">
-        <v>-0.01238869643154785</v>
+        <v>-0.01265916770636671</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.02673374286134971</v>
+        <v>0.02679402529576101</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.02673374286134971</v>
+        <v>0.02679402529576101</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.02673374286134971</v>
+        <v>0.02679402529576101</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.02673374286134971</v>
+        <v>0.02679402529576101</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.02673374286134971</v>
+        <v>0.02679402529576101</v>
       </c>
     </row>
     <row r="26">
@@ -2872,10 +2872,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.02919526129581045</v>
+        <v>0.02919772446390898</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.03294570301624859</v>
+        <v>-0.03293608346528963</v>
       </c>
       <c r="E26" t="n">
         <v>0.01870228145209126</v>
@@ -2890,10 +2890,10 @@
         <v>0.02160733478429339</v>
       </c>
       <c r="I26" t="n">
-        <v>0.008627545881101834</v>
+        <v>0.008615819672632787</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0009832490796603348</v>
+        <v>0.0009833591916647761</v>
       </c>
       <c r="K26" t="n">
         <v>-0.01913315894132635</v>
@@ -2926,37 +2926,37 @@
         <v>-0.02083307056132282</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.006536416293456651</v>
+        <v>-0.006549132837965313</v>
       </c>
       <c r="V26" t="n">
         <v>0.005333011605320463</v>
       </c>
       <c r="W26" t="n">
-        <v>-0.01732854414914176</v>
+        <v>-0.01732897307715892</v>
       </c>
       <c r="X26" t="n">
-        <v>-0.01698416448736658</v>
+        <v>-0.01663179311327172</v>
       </c>
       <c r="Y26" t="n">
         <v>0.01781725184869007</v>
       </c>
       <c r="Z26" t="n">
-        <v>-0.01527794701111788</v>
+        <v>-0.01495587602223504</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.02455593314223732</v>
+        <v>0.02453764629350584</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.02455593314223732</v>
+        <v>0.02453764629350584</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.02455593314223732</v>
+        <v>0.02453764629350584</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.02455593314223732</v>
+        <v>0.02453764629350584</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.02455593314223732</v>
+        <v>0.02453764629350584</v>
       </c>
     </row>
     <row r="27">
@@ -2967,10 +2967,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-0.002022032432881297</v>
+        <v>-0.002025954417038177</v>
       </c>
       <c r="D27" t="n">
-        <v>0.01167844634436668</v>
+        <v>0.01239200902626618</v>
       </c>
       <c r="E27" t="n">
         <v>-0.01295046944601877</v>
@@ -2985,10 +2985,10 @@
         <v>-0.01450509610020384</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.005010219656408785</v>
+        <v>-0.005006923400276935</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.01096370506623201</v>
+        <v>-0.01096392481024087</v>
       </c>
       <c r="K27" t="n">
         <v>0.01849347385973895</v>
@@ -3021,37 +3021,37 @@
         <v>0.01860890877635635</v>
       </c>
       <c r="U27" t="n">
-        <v>0.0006971986838879474</v>
+        <v>0.0006835421073416841</v>
       </c>
       <c r="V27" t="n">
         <v>0.000910893924435757</v>
       </c>
       <c r="W27" t="n">
-        <v>0.01198043875121755</v>
+        <v>0.01198194623927785</v>
       </c>
       <c r="X27" t="n">
-        <v>-0.01028806025152241</v>
+        <v>-0.01077358622294345</v>
       </c>
       <c r="Y27" t="n">
         <v>-0.01035245849409834</v>
       </c>
       <c r="Z27" t="n">
-        <v>-0.004335349517413979</v>
+        <v>-0.00466663852266554</v>
       </c>
       <c r="AA27" t="n">
-        <v>-0.004145202693808108</v>
+        <v>-0.004076972995078919</v>
       </c>
       <c r="AB27" t="n">
-        <v>-0.004145202693808108</v>
+        <v>-0.004076972995078919</v>
       </c>
       <c r="AC27" t="n">
-        <v>-0.004145202693808108</v>
+        <v>-0.004076972995078919</v>
       </c>
       <c r="AD27" t="n">
-        <v>-0.004145202693808108</v>
+        <v>-0.004076972995078919</v>
       </c>
       <c r="AE27" t="n">
-        <v>-0.004145202693808108</v>
+        <v>-0.004076972995078919</v>
       </c>
     </row>
     <row r="28">
@@ -3066,10 +3066,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.03294485574979422</v>
+        <v>-0.0329432275897291</v>
       </c>
       <c r="D28" t="n">
-        <v>0.01509571048145672</v>
+        <v>0.01538424400415938</v>
       </c>
       <c r="E28" t="n">
         <v>-0.07310553489222139</v>
@@ -3084,10 +3084,10 @@
         <v>-0.02523759172950367</v>
       </c>
       <c r="I28" t="n">
-        <v>0.02689437813177512</v>
+        <v>0.02689352901174116</v>
       </c>
       <c r="J28" t="n">
-        <v>0.005286426405233295</v>
+        <v>0.005286859077250747</v>
       </c>
       <c r="K28" t="n">
         <v>0.07276661110266444</v>
@@ -3120,37 +3120,37 @@
         <v>0.04013596461343858</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.0421428200217128</v>
+        <v>-0.04212103358884134</v>
       </c>
       <c r="V28" t="n">
         <v>-0.2582039162481566</v>
       </c>
       <c r="W28" t="n">
-        <v>0.9915875564315022</v>
+        <v>0.9915875604635022</v>
       </c>
       <c r="X28" t="n">
-        <v>0.05908048287521931</v>
+        <v>0.05943174285726971</v>
       </c>
       <c r="Y28" t="n">
         <v>-0.03886075086643003</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.05882800545712021</v>
+        <v>0.05891563080462522</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.02756193307047732</v>
+        <v>0.02751529914861196</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.02756193307047732</v>
+        <v>0.02751529914861196</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.02756193307047732</v>
+        <v>0.02751529914861196</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.02756193307047732</v>
+        <v>0.02751529914861196</v>
       </c>
       <c r="AE28" t="n">
-        <v>0.02756193307047732</v>
+        <v>0.02751529914861196</v>
       </c>
     </row>
     <row r="29">
@@ -3165,10 +3165,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.01631982564479302</v>
+        <v>-0.01631645287665811</v>
       </c>
       <c r="D29" t="n">
-        <v>0.02169669253095211</v>
+        <v>0.02382601537081698</v>
       </c>
       <c r="E29" t="n">
         <v>-0.01579043487161739</v>
@@ -3183,10 +3183,10 @@
         <v>-0.01669819343592773</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.0217306702132268</v>
+        <v>-0.02173889232555569</v>
       </c>
       <c r="J29" t="n">
-        <v>0.01480737021327008</v>
+        <v>0.0148070608052576</v>
       </c>
       <c r="K29" t="n">
         <v>-0.003829381689175267</v>
@@ -3219,37 +3219,37 @@
         <v>-0.001606776640271065</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.02056057887042315</v>
+        <v>-0.02056447090257884</v>
       </c>
       <c r="V29" t="n">
         <v>0.001894137291765491</v>
       </c>
       <c r="W29" t="n">
-        <v>0.02120143592005743</v>
+        <v>0.02120265809610632</v>
       </c>
       <c r="X29" t="n">
-        <v>0.01371350166854006</v>
+        <v>0.01333848398953936</v>
       </c>
       <c r="Y29" t="n">
         <v>0.001305189076207563</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.004752735166109407</v>
+        <v>0.004634531993381279</v>
       </c>
       <c r="AA29" t="n">
-        <v>-0.01936753037470121</v>
+        <v>-0.01932930970117239</v>
       </c>
       <c r="AB29" t="n">
-        <v>-0.01936753037470121</v>
+        <v>-0.01932930970117239</v>
       </c>
       <c r="AC29" t="n">
-        <v>-0.01936753037470121</v>
+        <v>-0.01932930970117239</v>
       </c>
       <c r="AD29" t="n">
-        <v>-0.01936753037470121</v>
+        <v>-0.01932930970117239</v>
       </c>
       <c r="AE29" t="n">
-        <v>-0.01936753037470121</v>
+        <v>-0.01932930970117239</v>
       </c>
     </row>
     <row r="30">
@@ -3264,10 +3264,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.005275888435035537</v>
+        <v>-0.00527955601918224</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.009876604242586988</v>
+        <v>-0.01083571843051021</v>
       </c>
       <c r="E30" t="n">
         <v>-0.0006444854657794185</v>
@@ -3282,10 +3282,10 @@
         <v>-0.01741705836068233</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.00766099979443999</v>
+        <v>-0.007655482098219282</v>
       </c>
       <c r="J30" t="n">
-        <v>0.002509547477225107</v>
+        <v>0.002509810325235709</v>
       </c>
       <c r="K30" t="n">
         <v>0.01605878771435151</v>
@@ -3318,37 +3318,37 @@
         <v>0.02752155642886225</v>
       </c>
       <c r="U30" t="n">
-        <v>0.0151290474531619</v>
+        <v>0.01510122550004902</v>
       </c>
       <c r="V30" t="n">
         <v>0.0587889477595579</v>
       </c>
       <c r="W30" t="n">
-        <v>0.1101223529168941</v>
+        <v>0.1101223846928954</v>
       </c>
       <c r="X30" t="n">
-        <v>-0.02076856095874244</v>
+        <v>-0.02120478420819136</v>
       </c>
       <c r="Y30" t="n">
         <v>-0.02759040955161638</v>
       </c>
       <c r="Z30" t="n">
-        <v>-0.006804691664187667</v>
+        <v>-0.006768186702727467</v>
       </c>
       <c r="AA30" t="n">
-        <v>-0.003641547217661888</v>
+        <v>-0.003603134160125366</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.003641547217661888</v>
+        <v>-0.003603134160125366</v>
       </c>
       <c r="AC30" t="n">
-        <v>-0.003641547217661888</v>
+        <v>-0.003603134160125366</v>
       </c>
       <c r="AD30" t="n">
-        <v>-0.003641547217661888</v>
+        <v>-0.003603134160125366</v>
       </c>
       <c r="AE30" t="n">
-        <v>-0.003641547217661888</v>
+        <v>-0.003603134160125366</v>
       </c>
     </row>
     <row r="31">
@@ -3363,10 +3363,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.004021122400844895</v>
+        <v>-0.004021729216869168</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.01057786368304562</v>
+        <v>-0.01011353770137278</v>
       </c>
       <c r="E31" t="n">
         <v>-0.004145227461809097</v>
@@ -3381,10 +3381,10 @@
         <v>-0.003690063891602556</v>
       </c>
       <c r="I31" t="n">
-        <v>0.01975008674200347</v>
+        <v>0.01975763416630536</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.01078861881916973</v>
+        <v>-0.01078844265916262</v>
       </c>
       <c r="K31" t="n">
         <v>0.009151257294050291</v>
@@ -3417,37 +3417,37 @@
         <v>0.005971506574860262</v>
       </c>
       <c r="U31" t="n">
-        <v>-0.002917972052718882</v>
+        <v>-0.002922716180908647</v>
       </c>
       <c r="V31" t="n">
         <v>-0.005945448237817929</v>
       </c>
       <c r="W31" t="n">
-        <v>0.01071685204467408</v>
+        <v>0.01071737524469501</v>
       </c>
       <c r="X31" t="n">
-        <v>0.004086961507478459</v>
+        <v>0.003925315933012636</v>
       </c>
       <c r="Y31" t="n">
         <v>-0.008818403392736134</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.01566260942650437</v>
+        <v>0.01571711582868463</v>
       </c>
       <c r="AA31" t="n">
-        <v>-0.002389504127580165</v>
+        <v>-0.002384411327376453</v>
       </c>
       <c r="AB31" t="n">
-        <v>-0.002389504127580165</v>
+        <v>-0.002384411327376453</v>
       </c>
       <c r="AC31" t="n">
-        <v>-0.002389504127580165</v>
+        <v>-0.002384411327376453</v>
       </c>
       <c r="AD31" t="n">
-        <v>-0.002389504127580165</v>
+        <v>-0.002384411327376453</v>
       </c>
       <c r="AE31" t="n">
-        <v>-0.002389504127580165</v>
+        <v>-0.002384411327376453</v>
       </c>
     </row>
     <row r="32">
@@ -3462,10 +3462,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.4481400481656019</v>
+        <v>0.4481359736374389</v>
       </c>
       <c r="D32" t="n">
-        <v>0.01120465278121782</v>
+        <v>0.01136347848734892</v>
       </c>
       <c r="E32" t="n">
         <v>0.9775172146846886</v>
@@ -3480,10 +3480,10 @@
         <v>0.9869956307758251</v>
       </c>
       <c r="I32" t="n">
-        <v>0.432798351391934</v>
+        <v>0.4328004160640166</v>
       </c>
       <c r="J32" t="n">
-        <v>0.0653274024910461</v>
+        <v>0.06532754389905181</v>
       </c>
       <c r="K32" t="n">
         <v>-0.492156328134253</v>
@@ -3516,37 +3516,37 @@
         <v>-0.5661943183597726</v>
       </c>
       <c r="U32" t="n">
-        <v>-0.1241749719109989</v>
+        <v>-0.1241711320068453</v>
       </c>
       <c r="V32" t="n">
         <v>-0.005861654826466192</v>
       </c>
       <c r="W32" t="n">
-        <v>-0.02247286841891473</v>
+        <v>-0.02247092845083714</v>
       </c>
       <c r="X32" t="n">
-        <v>-0.5920938360677533</v>
+        <v>-0.5920986247399449</v>
       </c>
       <c r="Y32" t="n">
         <v>0.02857771160710846</v>
       </c>
       <c r="Z32" t="n">
-        <v>-0.571453627978145</v>
+        <v>-0.5712066637442665</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.7441564047422561</v>
+        <v>0.7441460848378434</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.7441564047422561</v>
+        <v>0.7441460848378434</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.7441564047422561</v>
+        <v>0.7441460848378434</v>
       </c>
       <c r="AD32" t="n">
-        <v>0.7441564047422561</v>
+        <v>0.7441460848378434</v>
       </c>
       <c r="AE32" t="n">
-        <v>0.7441564047422561</v>
+        <v>0.7441460848378434</v>
       </c>
     </row>
     <row r="33">
@@ -3561,10 +3561,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.007136567901462715</v>
+        <v>-0.007136484861459393</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.02036975430304045</v>
+        <v>-0.02111131655546207</v>
       </c>
       <c r="E33" t="n">
         <v>-0.01410533173221327</v>
@@ -3579,10 +3579,10 @@
         <v>-0.006144108149764326</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01063213626528545</v>
+        <v>0.01063592884143715</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.02178099635055827</v>
+        <v>-0.02178075491054853</v>
       </c>
       <c r="K33" t="n">
         <v>0.008465578706623147</v>
@@ -3615,37 +3615,37 @@
         <v>0.005647403361896133</v>
       </c>
       <c r="U33" t="n">
-        <v>-0.0007886527995461119</v>
+        <v>-0.0008017073600682943</v>
       </c>
       <c r="V33" t="n">
         <v>-0.027352375142095</v>
       </c>
       <c r="W33" t="n">
-        <v>0.009694360323774411</v>
+        <v>0.009696022083840882</v>
       </c>
       <c r="X33" t="n">
-        <v>0.008645790201831606</v>
+        <v>0.00879183203167328</v>
       </c>
       <c r="Y33" t="n">
         <v>0.02070782530831301</v>
       </c>
       <c r="Z33" t="n">
-        <v>0.00959445331177813</v>
+        <v>0.009660871586434864</v>
       </c>
       <c r="AA33" t="n">
-        <v>-0.001027793417111737</v>
+        <v>-0.001018046536721861</v>
       </c>
       <c r="AB33" t="n">
-        <v>-0.001027793417111737</v>
+        <v>-0.001018046536721861</v>
       </c>
       <c r="AC33" t="n">
-        <v>-0.001027793417111737</v>
+        <v>-0.001018046536721861</v>
       </c>
       <c r="AD33" t="n">
-        <v>-0.001027793417111737</v>
+        <v>-0.001018046536721861</v>
       </c>
       <c r="AE33" t="n">
-        <v>-0.001027793417111737</v>
+        <v>-0.001018046536721861</v>
       </c>
     </row>
     <row r="34">
@@ -3660,10 +3660,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.0005329734933189396</v>
+        <v>-0.0005344434453777377</v>
       </c>
       <c r="D34" t="n">
-        <v>0.002493713890492887</v>
+        <v>0.004530915541276815</v>
       </c>
       <c r="E34" t="n">
         <v>0.00220429026417161</v>
@@ -3678,10 +3678,10 @@
         <v>0.00287552699502108</v>
       </c>
       <c r="I34" t="n">
-        <v>0.01860353940014157</v>
+        <v>0.01860427063217082</v>
       </c>
       <c r="J34" t="n">
-        <v>0.02213644538889566</v>
+        <v>0.02213655761290019</v>
       </c>
       <c r="K34" t="n">
         <v>0.03340589250423569</v>
@@ -3714,37 +3714,37 @@
         <v>0.03232792161311687</v>
       </c>
       <c r="U34" t="n">
-        <v>-0.01324678315387133</v>
+        <v>-0.01324563844982554</v>
       </c>
       <c r="V34" t="n">
         <v>-0.00665778977031159</v>
       </c>
       <c r="W34" t="n">
-        <v>-0.01312951185318047</v>
+        <v>-0.01312824782112991</v>
       </c>
       <c r="X34" t="n">
-        <v>-0.00459880175195207</v>
+        <v>-0.004624038232961529</v>
       </c>
       <c r="Y34" t="n">
         <v>0.0004177651367106054</v>
       </c>
       <c r="Z34" t="n">
-        <v>0.008185312455412498</v>
+        <v>0.008084604227384169</v>
       </c>
       <c r="AA34" t="n">
-        <v>0.02360878040035121</v>
+        <v>0.0236230075049203</v>
       </c>
       <c r="AB34" t="n">
-        <v>0.02360878040035121</v>
+        <v>0.0236230075049203</v>
       </c>
       <c r="AC34" t="n">
-        <v>0.02360878040035121</v>
+        <v>0.0236230075049203</v>
       </c>
       <c r="AD34" t="n">
-        <v>0.02360878040035121</v>
+        <v>0.0236230075049203</v>
       </c>
       <c r="AE34" t="n">
-        <v>0.02360878040035121</v>
+        <v>0.0236230075049203</v>
       </c>
     </row>
     <row r="35">
@@ -3759,10 +3759,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.03784245808969832</v>
+        <v>-0.03783795415351816</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.007522902711053979</v>
+        <v>-0.007122572944598662</v>
       </c>
       <c r="E35" t="n">
         <v>-0.03233770564550822</v>
@@ -3777,10 +3777,10 @@
         <v>-0.02476387635055505</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.01662850136914005</v>
+        <v>-0.01664051740162069</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0202765941138767</v>
+        <v>0.02027656790587564</v>
       </c>
       <c r="K35" t="n">
         <v>0.7698346114333843</v>
@@ -3813,37 +3813,37 @@
         <v>0.7723875800475031</v>
       </c>
       <c r="U35" t="n">
-        <v>0.004739360157574405</v>
+        <v>0.004751079358043173</v>
       </c>
       <c r="V35" t="n">
         <v>-0.02097465031098601</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.0006555291142211645</v>
+        <v>-0.0006572054662882185</v>
       </c>
       <c r="X35" t="n">
-        <v>0.03012534590901383</v>
+        <v>0.03044973856198954</v>
       </c>
       <c r="Y35" t="n">
         <v>0.01237743063909722</v>
       </c>
       <c r="Z35" t="n">
-        <v>0.01612751037310041</v>
+        <v>0.01603189091327563</v>
       </c>
       <c r="AA35" t="n">
-        <v>-0.1989899916395996</v>
+        <v>-0.1990154894326196</v>
       </c>
       <c r="AB35" t="n">
-        <v>-0.1989899916395996</v>
+        <v>-0.1990154894326196</v>
       </c>
       <c r="AC35" t="n">
-        <v>-0.1989899916395996</v>
+        <v>-0.1990154894326196</v>
       </c>
       <c r="AD35" t="n">
-        <v>-0.1989899916395996</v>
+        <v>-0.1990154894326196</v>
       </c>
       <c r="AE35" t="n">
-        <v>-0.1989899916395996</v>
+        <v>-0.1990154894326196</v>
       </c>
     </row>
     <row r="36">
@@ -3858,10 +3858,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.003370788902831556</v>
+        <v>-0.003370851974834078</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.008551209045857705</v>
+        <v>-0.009057641486250217</v>
       </c>
       <c r="E36" t="n">
         <v>0.0135509276780371</v>
@@ -3876,10 +3876,10 @@
         <v>0.0153446123897845</v>
       </c>
       <c r="I36" t="n">
-        <v>0.01010472165218886</v>
+        <v>0.0101025349641014</v>
       </c>
       <c r="J36" t="n">
-        <v>0.003765523879886171</v>
+        <v>0.003765316903877822</v>
       </c>
       <c r="K36" t="n">
         <v>-0.002919916340796654</v>
@@ -3912,37 +3912,37 @@
         <v>-0.001840691209627648</v>
       </c>
       <c r="U36" t="n">
-        <v>0.02551849849273994</v>
+        <v>0.02552703970908159</v>
       </c>
       <c r="V36" t="n">
         <v>0.003193437055737481</v>
       </c>
       <c r="W36" t="n">
-        <v>0.01623655332146213</v>
+        <v>0.01623732900149316</v>
       </c>
       <c r="X36" t="n">
-        <v>0.006782350063294001</v>
+        <v>0.006787543183501726</v>
       </c>
       <c r="Y36" t="n">
         <v>0.01057698138307926</v>
       </c>
       <c r="Z36" t="n">
-        <v>0.0002623263464930538</v>
+        <v>0.0002363343454533738</v>
       </c>
       <c r="AA36" t="n">
-        <v>0.001194354959774198</v>
+        <v>0.001188995471559819</v>
       </c>
       <c r="AB36" t="n">
-        <v>0.001194354959774198</v>
+        <v>0.001188995471559819</v>
       </c>
       <c r="AC36" t="n">
-        <v>0.001194354959774198</v>
+        <v>0.001188995471559819</v>
       </c>
       <c r="AD36" t="n">
-        <v>0.001194354959774198</v>
+        <v>0.001188995471559819</v>
       </c>
       <c r="AE36" t="n">
-        <v>0.001194354959774198</v>
+        <v>0.001188995471559819</v>
       </c>
     </row>
     <row r="37">
@@ -3957,10 +3957,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.002466315842652633</v>
+        <v>-0.002468153666726146</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.01817563616314932</v>
+        <v>-0.01849655195582338</v>
       </c>
       <c r="E37" t="n">
         <v>0.003466995690679827</v>
@@ -3975,10 +3975,10 @@
         <v>0.001163787598551504</v>
       </c>
       <c r="I37" t="n">
-        <v>0.008434503217380127</v>
+        <v>0.008439978961599157</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.008204052474918658</v>
+        <v>-0.008204083098919894</v>
       </c>
       <c r="K37" t="n">
         <v>0.0912124953604998</v>
@@ -4011,37 +4011,37 @@
         <v>0.09306873473074938</v>
       </c>
       <c r="U37" t="n">
-        <v>-0.005082317963292718</v>
+        <v>-0.00506757927470317</v>
       </c>
       <c r="V37" t="n">
         <v>0.005651380930055236</v>
       </c>
       <c r="W37" t="n">
-        <v>-0.001549531549981262</v>
+        <v>-0.001549547965981918</v>
       </c>
       <c r="X37" t="n">
-        <v>0.004658308122332325</v>
+        <v>0.004524600756984029</v>
       </c>
       <c r="Y37" t="n">
         <v>-0.01636277518251101</v>
       </c>
       <c r="Z37" t="n">
-        <v>0.001380982615239304</v>
+        <v>0.001376279191051168</v>
       </c>
       <c r="AA37" t="n">
-        <v>0.07671991919679676</v>
+        <v>0.07670306956412277</v>
       </c>
       <c r="AB37" t="n">
-        <v>0.07671991919679676</v>
+        <v>0.07670306956412277</v>
       </c>
       <c r="AC37" t="n">
-        <v>0.07671991919679676</v>
+        <v>0.07670306956412277</v>
       </c>
       <c r="AD37" t="n">
-        <v>0.07671991919679676</v>
+        <v>0.07670306956412277</v>
       </c>
       <c r="AE37" t="n">
-        <v>0.07671991919679676</v>
+        <v>0.07670306956412277</v>
       </c>
     </row>
     <row r="38">
@@ -4056,10 +4056,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.0009385289655411585</v>
+        <v>0.0009386339895453595</v>
       </c>
       <c r="D38" t="n">
-        <v>0.004448246416409761</v>
+        <v>0.002506160913642654</v>
       </c>
       <c r="E38" t="n">
         <v>-0.01580059042402361</v>
@@ -4074,10 +4074,10 @@
         <v>-0.01529779539591181</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.02557521068700842</v>
+        <v>-0.02557195436687817</v>
       </c>
       <c r="J38" t="n">
-        <v>-0.007364111289038792</v>
+        <v>-0.007363994937034099</v>
       </c>
       <c r="K38" t="n">
         <v>0.01900188172007527</v>
@@ -4110,37 +4110,37 @@
         <v>0.01925309846612394</v>
       </c>
       <c r="U38" t="n">
-        <v>0.00889409901176396</v>
+        <v>0.008851641954065678</v>
       </c>
       <c r="V38" t="n">
         <v>-0.004906690468267618</v>
       </c>
       <c r="W38" t="n">
-        <v>0.001505320572212823</v>
+        <v>0.001503448284137931</v>
       </c>
       <c r="X38" t="n">
-        <v>0.01969514469180578</v>
+        <v>0.01908037401121496</v>
       </c>
       <c r="Y38" t="n">
         <v>-0.008279627179185086</v>
       </c>
       <c r="Z38" t="n">
-        <v>0.01264958805798352</v>
+        <v>0.0125197401807896</v>
       </c>
       <c r="AA38" t="n">
-        <v>-0.0196732325949293</v>
+        <v>-0.01959914190396567</v>
       </c>
       <c r="AB38" t="n">
-        <v>-0.0196732325949293</v>
+        <v>-0.01959914190396567</v>
       </c>
       <c r="AC38" t="n">
-        <v>-0.0196732325949293</v>
+        <v>-0.01959914190396567</v>
       </c>
       <c r="AD38" t="n">
-        <v>-0.0196732325949293</v>
+        <v>-0.01959914190396567</v>
       </c>
       <c r="AE38" t="n">
-        <v>-0.0196732325949293</v>
+        <v>-0.01959914190396567</v>
       </c>
     </row>
     <row r="39">
@@ -4155,10 +4155,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.01436291558251662</v>
+        <v>0.01436507318260292</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.02354107280193862</v>
+        <v>-0.02168263115146386</v>
       </c>
       <c r="E39" t="n">
         <v>0.003517886540715461</v>
@@ -4173,10 +4173,10 @@
         <v>-0.00346554925862197</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.01402935684917427</v>
+        <v>-0.01403307310532292</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.001699731572560372</v>
+        <v>-0.001699571252553906</v>
       </c>
       <c r="K39" t="n">
         <v>0.04638799231951969</v>
@@ -4209,37 +4209,37 @@
         <v>0.04929666369986654</v>
       </c>
       <c r="U39" t="n">
-        <v>0.01431934982077399</v>
+        <v>0.01431525071661003</v>
       </c>
       <c r="V39" t="n">
         <v>0.01925972957038918</v>
       </c>
       <c r="W39" t="n">
-        <v>0.006667095050683801</v>
+        <v>0.006669502922780115</v>
       </c>
       <c r="X39" t="n">
-        <v>-0.01812588072503523</v>
+        <v>-0.01789422407576896</v>
       </c>
       <c r="Y39" t="n">
         <v>-0.02660734666429386</v>
       </c>
       <c r="Z39" t="n">
-        <v>-0.01535850608634024</v>
+        <v>-0.01504424719376989</v>
       </c>
       <c r="AA39" t="n">
-        <v>0.006397080639883226</v>
+        <v>0.006371701598868063</v>
       </c>
       <c r="AB39" t="n">
-        <v>0.006397080639883226</v>
+        <v>0.006371701598868063</v>
       </c>
       <c r="AC39" t="n">
-        <v>0.006397080639883226</v>
+        <v>0.006371701598868063</v>
       </c>
       <c r="AD39" t="n">
-        <v>0.006397080639883226</v>
+        <v>0.006371701598868063</v>
       </c>
       <c r="AE39" t="n">
-        <v>0.006397080639883226</v>
+        <v>0.006371701598868063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>